<commit_message>
Change some variables Add Standard Deviation calculation, GPA Trend analysis, and Linear Regression implementation to KNN Logic
</commit_message>
<xml_diff>
--- a/data/Dataset IPK Mahasiswa.xlsx
+++ b/data/Dataset IPK Mahasiswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Malas Ngoding\PI-MachineLearning\webApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F249AA-E63B-4EAA-A8FF-73762A7187BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F5FCCD-DFAD-47B8-A252-EF40CBF63998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FEB538D4-D2EB-469D-9498-4E67ED4ACCC5}"/>
   </bookViews>
@@ -149,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -174,14 +174,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -220,12 +225,6 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -245,20 +244,20 @@
     <tableColumn id="1" xr3:uid="{911922A4-D692-4C0D-85B1-7C0029FB1563}" name="MAHASISWA" dataDxfId="10" dataCellStyle="Normal">
       <calculatedColumnFormula>"Mahasiswa " &amp; ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{36BE6329-D390-4CAD-91F7-F799DF2EDD1B}" name="SEMESTER 1" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{6C6AED49-C2E4-4622-A54E-D5B58F3086DB}" name="SEMESTER 2" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{A792822B-A1D8-4B99-802F-3E357F59BB18}" name="SEMESTER 3" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{F2F36FB0-B352-4B1E-ACB8-22EA9B15B020}" name="SEMESTER 4" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{D8128881-09B1-4E9D-BD29-1F6F85266BC6}" name="SEMESTER 5" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{9C7A6035-CB6B-4348-9202-0B0A92E84DF5}" name="SEMESTER 6" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{D0C58422-E9C7-4239-8EF0-A8B0B8152E2D}" name="SEMESTER 7" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{94014B41-28AB-4E91-8CDB-0C3556E678D2}" name="RATA-RATA IPK" dataDxfId="0" dataCellStyle="Normal">
+    <tableColumn id="2" xr3:uid="{36BE6329-D390-4CAD-91F7-F799DF2EDD1B}" name="SEMESTER 1" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{6C6AED49-C2E4-4622-A54E-D5B58F3086DB}" name="SEMESTER 2" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{A792822B-A1D8-4B99-802F-3E357F59BB18}" name="SEMESTER 3" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{F2F36FB0-B352-4B1E-ACB8-22EA9B15B020}" name="SEMESTER 4" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{D8128881-09B1-4E9D-BD29-1F6F85266BC6}" name="SEMESTER 5" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{9C7A6035-CB6B-4348-9202-0B0A92E84DF5}" name="SEMESTER 6" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{D0C58422-E9C7-4239-8EF0-A8B0B8152E2D}" name="SEMESTER 7" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{94014B41-28AB-4E91-8CDB-0C3556E678D2}" name="RATA-RATA IPK" dataDxfId="2" dataCellStyle="Normal">
       <calculatedColumnFormula>ROUND(AVERAGE(B3,C3,D3,E3,F3,G3,H3),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1EBD481C-BC38-4BEB-959B-CF4A9B6938E6}" name="RANK" dataDxfId="9" dataCellStyle="Normal">
-      <calculatedColumnFormula array="1">_xlfn.IFS(I3&gt;=3.7,"A",I3&gt;=3.3,"B",I3&gt;=2.9,"C",I3&gt;=2.6,"D",I3&lt;=2.5,"E")</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{1EBD481C-BC38-4BEB-959B-CF4A9B6938E6}" name="RANK" dataDxfId="1" dataCellStyle="Normal">
+      <calculatedColumnFormula array="1">_xlfn.IFS(I3&gt;=3.7,"A",I3&gt;=3.3,"B",I3&gt;=2.8,"C",I3&gt;=2.5,"D",I3&lt;=2.4,"E")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4E433DCE-F9F6-4A91-B5F2-B0414E7B35D8}" name="STATUS" dataDxfId="8" dataCellStyle="Normal">
+    <tableColumn id="11" xr3:uid="{4E433DCE-F9F6-4A91-B5F2-B0414E7B35D8}" name="STATUS" dataDxfId="0" dataCellStyle="Normal">
       <calculatedColumnFormula array="1">_xlfn.IFS(J3="A","LULUS",J3="B","LULUS",J3="C","LULUS",J3="D","TIDAK LULUS",J3="E","TIDAK LULUS")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -565,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDF0E10-E7F5-48B4-8586-200673539952}">
   <dimension ref="A1:V567"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A224" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K184" sqref="K184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,25 +631,25 @@
         <f t="shared" ref="A2:A66" si="0">"Mahasiswa " &amp; ROW()-1</f>
         <v>Mahasiswa 1</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="7">
         <v>4</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="7">
         <v>4</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="7">
         <v>3.95</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="7">
         <v>4</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="7">
         <v>4</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="7">
         <v>4</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>3.8</v>
       </c>
       <c r="I2" s="7">
@@ -697,7 +696,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="9" t="str" cm="1">
-        <f t="array" ref="J3">_xlfn.IFS(I3&gt;=3.7,"A",I3&gt;=3.3,"B",I3&gt;=2.9,"C",I3&gt;=2.6,"D",I3&lt;=2.5,"E")</f>
+        <f t="array" ref="J3">_xlfn.IFS(I3&gt;=3.7,"A",I3&gt;=3.3,"B",I3&gt;=2.8,"C",I3&gt;=2.5,"D",I3&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K3" s="9" t="str" cm="1">
@@ -736,7 +735,7 @@
         <v>4</v>
       </c>
       <c r="J4" s="9" t="str" cm="1">
-        <f t="array" ref="J4">_xlfn.IFS(I4&gt;=3.7,"A",I4&gt;=3.3,"B",I4&gt;=2.9,"C",I4&gt;=2.6,"D",I4&lt;=2.5,"E")</f>
+        <f t="array" ref="J4">_xlfn.IFS(I4&gt;=3.7,"A",I4&gt;=3.3,"B",I4&gt;=2.8,"C",I4&gt;=2.5,"D",I4&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K4" s="9" t="str" cm="1">
@@ -775,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="9" t="str" cm="1">
-        <f t="array" ref="J5">_xlfn.IFS(I5&gt;=3.7,"A",I5&gt;=3.3,"B",I5&gt;=2.9,"C",I5&gt;=2.6,"D",I5&lt;=2.5,"E")</f>
+        <f t="array" ref="J5">_xlfn.IFS(I5&gt;=3.7,"A",I5&gt;=3.3,"B",I5&gt;=2.8,"C",I5&gt;=2.5,"D",I5&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K5" s="9" t="str" cm="1">
@@ -814,7 +813,7 @@
         <v>3.9</v>
       </c>
       <c r="J6" s="9" t="str" cm="1">
-        <f t="array" ref="J6">_xlfn.IFS(I6&gt;=3.7,"A",I6&gt;=3.3,"B",I6&gt;=2.9,"C",I6&gt;=2.6,"D",I6&lt;=2.5,"E")</f>
+        <f t="array" ref="J6">_xlfn.IFS(I6&gt;=3.7,"A",I6&gt;=3.3,"B",I6&gt;=2.8,"C",I6&gt;=2.5,"D",I6&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K6" s="9" t="str" cm="1">
@@ -853,7 +852,7 @@
         <v>3.9</v>
       </c>
       <c r="J7" s="9" t="str" cm="1">
-        <f t="array" ref="J7">_xlfn.IFS(I7&gt;=3.7,"A",I7&gt;=3.3,"B",I7&gt;=2.9,"C",I7&gt;=2.6,"D",I7&lt;=2.5,"E")</f>
+        <f t="array" ref="J7">_xlfn.IFS(I7&gt;=3.7,"A",I7&gt;=3.3,"B",I7&gt;=2.8,"C",I7&gt;=2.5,"D",I7&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K7" s="9" t="str" cm="1">
@@ -892,7 +891,7 @@
         <v>3.9</v>
       </c>
       <c r="J8" s="9" t="str" cm="1">
-        <f t="array" ref="J8">_xlfn.IFS(I8&gt;=3.7,"A",I8&gt;=3.3,"B",I8&gt;=2.9,"C",I8&gt;=2.6,"D",I8&lt;=2.5,"E")</f>
+        <f t="array" ref="J8">_xlfn.IFS(I8&gt;=3.7,"A",I8&gt;=3.3,"B",I8&gt;=2.8,"C",I8&gt;=2.5,"D",I8&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K8" s="9" t="str" cm="1">
@@ -931,7 +930,7 @@
         <v>3.9</v>
       </c>
       <c r="J9" s="9" t="str" cm="1">
-        <f t="array" ref="J9">_xlfn.IFS(I9&gt;=3.7,"A",I9&gt;=3.3,"B",I9&gt;=2.9,"C",I9&gt;=2.6,"D",I9&lt;=2.5,"E")</f>
+        <f t="array" ref="J9">_xlfn.IFS(I9&gt;=3.7,"A",I9&gt;=3.3,"B",I9&gt;=2.8,"C",I9&gt;=2.5,"D",I9&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K9" s="9" t="str" cm="1">
@@ -970,7 +969,7 @@
         <v>3.9</v>
       </c>
       <c r="J10" s="9" t="str" cm="1">
-        <f t="array" ref="J10">_xlfn.IFS(I10&gt;=3.7,"A",I10&gt;=3.3,"B",I10&gt;=2.9,"C",I10&gt;=2.6,"D",I10&lt;=2.5,"E")</f>
+        <f t="array" ref="J10">_xlfn.IFS(I10&gt;=3.7,"A",I10&gt;=3.3,"B",I10&gt;=2.8,"C",I10&gt;=2.5,"D",I10&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K10" s="9" t="str" cm="1">
@@ -1009,7 +1008,7 @@
         <v>3.9</v>
       </c>
       <c r="J11" s="9" t="str" cm="1">
-        <f t="array" ref="J11">_xlfn.IFS(I11&gt;=3.7,"A",I11&gt;=3.3,"B",I11&gt;=2.9,"C",I11&gt;=2.6,"D",I11&lt;=2.5,"E")</f>
+        <f t="array" ref="J11">_xlfn.IFS(I11&gt;=3.7,"A",I11&gt;=3.3,"B",I11&gt;=2.8,"C",I11&gt;=2.5,"D",I11&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K11" s="9" t="str" cm="1">
@@ -1048,7 +1047,7 @@
         <v>3.8</v>
       </c>
       <c r="J12" s="9" t="str" cm="1">
-        <f t="array" ref="J12">_xlfn.IFS(I12&gt;=3.7,"A",I12&gt;=3.3,"B",I12&gt;=2.9,"C",I12&gt;=2.6,"D",I12&lt;=2.5,"E")</f>
+        <f t="array" ref="J12">_xlfn.IFS(I12&gt;=3.7,"A",I12&gt;=3.3,"B",I12&gt;=2.8,"C",I12&gt;=2.5,"D",I12&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K12" s="9" t="str" cm="1">
@@ -1089,7 +1088,7 @@
         <v>3.8</v>
       </c>
       <c r="J13" s="9" t="str" cm="1">
-        <f t="array" ref="J13">_xlfn.IFS(I13&gt;=3.7,"A",I13&gt;=3.3,"B",I13&gt;=2.9,"C",I13&gt;=2.6,"D",I13&lt;=2.5,"E")</f>
+        <f t="array" ref="J13">_xlfn.IFS(I13&gt;=3.7,"A",I13&gt;=3.3,"B",I13&gt;=2.8,"C",I13&gt;=2.5,"D",I13&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K13" s="9" t="str" cm="1">
@@ -1130,7 +1129,7 @@
         <v>3.8</v>
       </c>
       <c r="J14" s="9" t="str" cm="1">
-        <f t="array" ref="J14">_xlfn.IFS(I14&gt;=3.7,"A",I14&gt;=3.3,"B",I14&gt;=2.9,"C",I14&gt;=2.6,"D",I14&lt;=2.5,"E")</f>
+        <f t="array" ref="J14">_xlfn.IFS(I14&gt;=3.7,"A",I14&gt;=3.3,"B",I14&gt;=2.8,"C",I14&gt;=2.5,"D",I14&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K14" s="9" t="str" cm="1">
@@ -1171,7 +1170,7 @@
         <v>3.8</v>
       </c>
       <c r="J15" s="9" t="str" cm="1">
-        <f t="array" ref="J15">_xlfn.IFS(I15&gt;=3.7,"A",I15&gt;=3.3,"B",I15&gt;=2.9,"C",I15&gt;=2.6,"D",I15&lt;=2.5,"E")</f>
+        <f t="array" ref="J15">_xlfn.IFS(I15&gt;=3.7,"A",I15&gt;=3.3,"B",I15&gt;=2.8,"C",I15&gt;=2.5,"D",I15&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K15" s="9" t="str" cm="1">
@@ -1212,7 +1211,7 @@
         <v>3.8</v>
       </c>
       <c r="J16" s="9" t="str" cm="1">
-        <f t="array" ref="J16">_xlfn.IFS(I16&gt;=3.7,"A",I16&gt;=3.3,"B",I16&gt;=2.9,"C",I16&gt;=2.6,"D",I16&lt;=2.5,"E")</f>
+        <f t="array" ref="J16">_xlfn.IFS(I16&gt;=3.7,"A",I16&gt;=3.3,"B",I16&gt;=2.8,"C",I16&gt;=2.5,"D",I16&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K16" s="9" t="str" cm="1">
@@ -1253,7 +1252,7 @@
         <v>3.7</v>
       </c>
       <c r="J17" s="9" t="str" cm="1">
-        <f t="array" ref="J17">_xlfn.IFS(I17&gt;=3.7,"A",I17&gt;=3.3,"B",I17&gt;=2.9,"C",I17&gt;=2.6,"D",I17&lt;=2.5,"E")</f>
+        <f t="array" ref="J17">_xlfn.IFS(I17&gt;=3.7,"A",I17&gt;=3.3,"B",I17&gt;=2.8,"C",I17&gt;=2.5,"D",I17&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K17" s="9" t="str" cm="1">
@@ -1294,7 +1293,7 @@
         <v>3.7</v>
       </c>
       <c r="J18" s="9" t="str" cm="1">
-        <f t="array" ref="J18">_xlfn.IFS(I18&gt;=3.7,"A",I18&gt;=3.3,"B",I18&gt;=2.9,"C",I18&gt;=2.6,"D",I18&lt;=2.5,"E")</f>
+        <f t="array" ref="J18">_xlfn.IFS(I18&gt;=3.7,"A",I18&gt;=3.3,"B",I18&gt;=2.8,"C",I18&gt;=2.5,"D",I18&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K18" s="9" t="str" cm="1">
@@ -1335,7 +1334,7 @@
         <v>3.7</v>
       </c>
       <c r="J19" s="9" t="str" cm="1">
-        <f t="array" ref="J19">_xlfn.IFS(I19&gt;=3.7,"A",I19&gt;=3.3,"B",I19&gt;=2.9,"C",I19&gt;=2.6,"D",I19&lt;=2.5,"E")</f>
+        <f t="array" ref="J19">_xlfn.IFS(I19&gt;=3.7,"A",I19&gt;=3.3,"B",I19&gt;=2.8,"C",I19&gt;=2.5,"D",I19&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K19" s="9" t="str" cm="1">
@@ -1376,7 +1375,7 @@
         <v>3.7</v>
       </c>
       <c r="J20" s="9" t="str" cm="1">
-        <f t="array" ref="J20">_xlfn.IFS(I20&gt;=3.7,"A",I20&gt;=3.3,"B",I20&gt;=2.9,"C",I20&gt;=2.6,"D",I20&lt;=2.5,"E")</f>
+        <f t="array" ref="J20">_xlfn.IFS(I20&gt;=3.7,"A",I20&gt;=3.3,"B",I20&gt;=2.8,"C",I20&gt;=2.5,"D",I20&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K20" s="9" t="str" cm="1">
@@ -1417,7 +1416,7 @@
         <v>3.7</v>
       </c>
       <c r="J21" s="9" t="str" cm="1">
-        <f t="array" ref="J21">_xlfn.IFS(I21&gt;=3.7,"A",I21&gt;=3.3,"B",I21&gt;=2.9,"C",I21&gt;=2.6,"D",I21&lt;=2.5,"E")</f>
+        <f t="array" ref="J21">_xlfn.IFS(I21&gt;=3.7,"A",I21&gt;=3.3,"B",I21&gt;=2.8,"C",I21&gt;=2.5,"D",I21&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K21" s="9" t="str" cm="1">
@@ -1458,7 +1457,7 @@
         <v>3.7</v>
       </c>
       <c r="J22" s="9" t="str" cm="1">
-        <f t="array" ref="J22">_xlfn.IFS(I22&gt;=3.7,"A",I22&gt;=3.3,"B",I22&gt;=2.9,"C",I22&gt;=2.6,"D",I22&lt;=2.5,"E")</f>
+        <f t="array" ref="J22">_xlfn.IFS(I22&gt;=3.7,"A",I22&gt;=3.3,"B",I22&gt;=2.8,"C",I22&gt;=2.5,"D",I22&lt;=2.4,"E")</f>
         <v>A</v>
       </c>
       <c r="K22" s="9" t="str" cm="1">
@@ -1499,7 +1498,7 @@
         <v>3.6</v>
       </c>
       <c r="J23" s="9" t="str" cm="1">
-        <f t="array" ref="J23">_xlfn.IFS(I23&gt;=3.7,"A",I23&gt;=3.3,"B",I23&gt;=2.9,"C",I23&gt;=2.6,"D",I23&lt;=2.5,"E")</f>
+        <f t="array" ref="J23">_xlfn.IFS(I23&gt;=3.7,"A",I23&gt;=3.3,"B",I23&gt;=2.8,"C",I23&gt;=2.5,"D",I23&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K23" s="9" t="str" cm="1">
@@ -1540,7 +1539,7 @@
         <v>3.6</v>
       </c>
       <c r="J24" s="9" t="str" cm="1">
-        <f t="array" ref="J24">_xlfn.IFS(I24&gt;=3.7,"A",I24&gt;=3.3,"B",I24&gt;=2.9,"C",I24&gt;=2.6,"D",I24&lt;=2.5,"E")</f>
+        <f t="array" ref="J24">_xlfn.IFS(I24&gt;=3.7,"A",I24&gt;=3.3,"B",I24&gt;=2.8,"C",I24&gt;=2.5,"D",I24&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K24" s="9" t="str" cm="1">
@@ -1581,7 +1580,7 @@
         <v>3.6</v>
       </c>
       <c r="J25" s="9" t="str" cm="1">
-        <f t="array" ref="J25">_xlfn.IFS(I25&gt;=3.7,"A",I25&gt;=3.3,"B",I25&gt;=2.9,"C",I25&gt;=2.6,"D",I25&lt;=2.5,"E")</f>
+        <f t="array" ref="J25">_xlfn.IFS(I25&gt;=3.7,"A",I25&gt;=3.3,"B",I25&gt;=2.8,"C",I25&gt;=2.5,"D",I25&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K25" s="9" t="str" cm="1">
@@ -1622,7 +1621,7 @@
         <v>3.6</v>
       </c>
       <c r="J26" s="9" t="str" cm="1">
-        <f t="array" ref="J26">_xlfn.IFS(I26&gt;=3.7,"A",I26&gt;=3.3,"B",I26&gt;=2.9,"C",I26&gt;=2.6,"D",I26&lt;=2.5,"E")</f>
+        <f t="array" ref="J26">_xlfn.IFS(I26&gt;=3.7,"A",I26&gt;=3.3,"B",I26&gt;=2.8,"C",I26&gt;=2.5,"D",I26&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K26" s="9" t="str" cm="1">
@@ -1663,7 +1662,7 @@
         <v>3.6</v>
       </c>
       <c r="J27" s="9" t="str" cm="1">
-        <f t="array" ref="J27">_xlfn.IFS(I27&gt;=3.7,"A",I27&gt;=3.3,"B",I27&gt;=2.9,"C",I27&gt;=2.6,"D",I27&lt;=2.5,"E")</f>
+        <f t="array" ref="J27">_xlfn.IFS(I27&gt;=3.7,"A",I27&gt;=3.3,"B",I27&gt;=2.8,"C",I27&gt;=2.5,"D",I27&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K27" s="9" t="str" cm="1">
@@ -1704,7 +1703,7 @@
         <v>3.6</v>
       </c>
       <c r="J28" s="9" t="str" cm="1">
-        <f t="array" ref="J28">_xlfn.IFS(I28&gt;=3.7,"A",I28&gt;=3.3,"B",I28&gt;=2.9,"C",I28&gt;=2.6,"D",I28&lt;=2.5,"E")</f>
+        <f t="array" ref="J28">_xlfn.IFS(I28&gt;=3.7,"A",I28&gt;=3.3,"B",I28&gt;=2.8,"C",I28&gt;=2.5,"D",I28&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K28" s="9" t="str" cm="1">
@@ -1745,7 +1744,7 @@
         <v>3.6</v>
       </c>
       <c r="J29" s="9" t="str" cm="1">
-        <f t="array" ref="J29">_xlfn.IFS(I29&gt;=3.7,"A",I29&gt;=3.3,"B",I29&gt;=2.9,"C",I29&gt;=2.6,"D",I29&lt;=2.5,"E")</f>
+        <f t="array" ref="J29">_xlfn.IFS(I29&gt;=3.7,"A",I29&gt;=3.3,"B",I29&gt;=2.8,"C",I29&gt;=2.5,"D",I29&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K29" s="9" t="str" cm="1">
@@ -1786,7 +1785,7 @@
         <v>3.6</v>
       </c>
       <c r="J30" s="9" t="str" cm="1">
-        <f t="array" ref="J30">_xlfn.IFS(I30&gt;=3.7,"A",I30&gt;=3.3,"B",I30&gt;=2.9,"C",I30&gt;=2.6,"D",I30&lt;=2.5,"E")</f>
+        <f t="array" ref="J30">_xlfn.IFS(I30&gt;=3.7,"A",I30&gt;=3.3,"B",I30&gt;=2.8,"C",I30&gt;=2.5,"D",I30&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K30" s="9" t="str" cm="1">
@@ -1827,7 +1826,7 @@
         <v>3.5</v>
       </c>
       <c r="J31" s="9" t="str" cm="1">
-        <f t="array" ref="J31">_xlfn.IFS(I31&gt;=3.7,"A",I31&gt;=3.3,"B",I31&gt;=2.9,"C",I31&gt;=2.6,"D",I31&lt;=2.5,"E")</f>
+        <f t="array" ref="J31">_xlfn.IFS(I31&gt;=3.7,"A",I31&gt;=3.3,"B",I31&gt;=2.8,"C",I31&gt;=2.5,"D",I31&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K31" s="9" t="str" cm="1">
@@ -1868,7 +1867,7 @@
         <v>3.5</v>
       </c>
       <c r="J32" s="9" t="str" cm="1">
-        <f t="array" ref="J32">_xlfn.IFS(I32&gt;=3.7,"A",I32&gt;=3.3,"B",I32&gt;=2.9,"C",I32&gt;=2.6,"D",I32&lt;=2.5,"E")</f>
+        <f t="array" ref="J32">_xlfn.IFS(I32&gt;=3.7,"A",I32&gt;=3.3,"B",I32&gt;=2.8,"C",I32&gt;=2.5,"D",I32&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K32" s="9" t="str" cm="1">
@@ -1909,7 +1908,7 @@
         <v>3.5</v>
       </c>
       <c r="J33" s="9" t="str" cm="1">
-        <f t="array" ref="J33">_xlfn.IFS(I33&gt;=3.7,"A",I33&gt;=3.3,"B",I33&gt;=2.9,"C",I33&gt;=2.6,"D",I33&lt;=2.5,"E")</f>
+        <f t="array" ref="J33">_xlfn.IFS(I33&gt;=3.7,"A",I33&gt;=3.3,"B",I33&gt;=2.8,"C",I33&gt;=2.5,"D",I33&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K33" s="9" t="str" cm="1">
@@ -1950,7 +1949,7 @@
         <v>3.5</v>
       </c>
       <c r="J34" s="9" t="str" cm="1">
-        <f t="array" ref="J34">_xlfn.IFS(I34&gt;=3.7,"A",I34&gt;=3.3,"B",I34&gt;=2.9,"C",I34&gt;=2.6,"D",I34&lt;=2.5,"E")</f>
+        <f t="array" ref="J34">_xlfn.IFS(I34&gt;=3.7,"A",I34&gt;=3.3,"B",I34&gt;=2.8,"C",I34&gt;=2.5,"D",I34&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K34" s="9" t="str" cm="1">
@@ -1991,7 +1990,7 @@
         <v>3.5</v>
       </c>
       <c r="J35" s="9" t="str" cm="1">
-        <f t="array" ref="J35">_xlfn.IFS(I35&gt;=3.7,"A",I35&gt;=3.3,"B",I35&gt;=2.9,"C",I35&gt;=2.6,"D",I35&lt;=2.5,"E")</f>
+        <f t="array" ref="J35">_xlfn.IFS(I35&gt;=3.7,"A",I35&gt;=3.3,"B",I35&gt;=2.8,"C",I35&gt;=2.5,"D",I35&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K35" s="9" t="str" cm="1">
@@ -2032,7 +2031,7 @@
         <v>3.5</v>
       </c>
       <c r="J36" s="9" t="str" cm="1">
-        <f t="array" ref="J36">_xlfn.IFS(I36&gt;=3.7,"A",I36&gt;=3.3,"B",I36&gt;=2.9,"C",I36&gt;=2.6,"D",I36&lt;=2.5,"E")</f>
+        <f t="array" ref="J36">_xlfn.IFS(I36&gt;=3.7,"A",I36&gt;=3.3,"B",I36&gt;=2.8,"C",I36&gt;=2.5,"D",I36&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K36" s="9" t="str" cm="1">
@@ -2073,7 +2072,7 @@
         <v>3.5</v>
       </c>
       <c r="J37" s="9" t="str" cm="1">
-        <f t="array" ref="J37">_xlfn.IFS(I37&gt;=3.7,"A",I37&gt;=3.3,"B",I37&gt;=2.9,"C",I37&gt;=2.6,"D",I37&lt;=2.5,"E")</f>
+        <f t="array" ref="J37">_xlfn.IFS(I37&gt;=3.7,"A",I37&gt;=3.3,"B",I37&gt;=2.8,"C",I37&gt;=2.5,"D",I37&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K37" s="9" t="str" cm="1">
@@ -2114,7 +2113,7 @@
         <v>3.5</v>
       </c>
       <c r="J38" s="9" t="str" cm="1">
-        <f t="array" ref="J38">_xlfn.IFS(I38&gt;=3.7,"A",I38&gt;=3.3,"B",I38&gt;=2.9,"C",I38&gt;=2.6,"D",I38&lt;=2.5,"E")</f>
+        <f t="array" ref="J38">_xlfn.IFS(I38&gt;=3.7,"A",I38&gt;=3.3,"B",I38&gt;=2.8,"C",I38&gt;=2.5,"D",I38&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K38" s="9" t="str" cm="1">
@@ -2155,7 +2154,7 @@
         <v>3.4</v>
       </c>
       <c r="J39" s="9" t="str" cm="1">
-        <f t="array" ref="J39">_xlfn.IFS(I39&gt;=3.7,"A",I39&gt;=3.3,"B",I39&gt;=2.9,"C",I39&gt;=2.6,"D",I39&lt;=2.5,"E")</f>
+        <f t="array" ref="J39">_xlfn.IFS(I39&gt;=3.7,"A",I39&gt;=3.3,"B",I39&gt;=2.8,"C",I39&gt;=2.5,"D",I39&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K39" s="9" t="str" cm="1">
@@ -2196,7 +2195,7 @@
         <v>3.4</v>
       </c>
       <c r="J40" s="9" t="str" cm="1">
-        <f t="array" ref="J40">_xlfn.IFS(I40&gt;=3.7,"A",I40&gt;=3.3,"B",I40&gt;=2.9,"C",I40&gt;=2.6,"D",I40&lt;=2.5,"E")</f>
+        <f t="array" ref="J40">_xlfn.IFS(I40&gt;=3.7,"A",I40&gt;=3.3,"B",I40&gt;=2.8,"C",I40&gt;=2.5,"D",I40&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K40" s="9" t="str" cm="1">
@@ -2237,7 +2236,7 @@
         <v>3.4</v>
       </c>
       <c r="J41" s="9" t="str" cm="1">
-        <f t="array" ref="J41">_xlfn.IFS(I41&gt;=3.7,"A",I41&gt;=3.3,"B",I41&gt;=2.9,"C",I41&gt;=2.6,"D",I41&lt;=2.5,"E")</f>
+        <f t="array" ref="J41">_xlfn.IFS(I41&gt;=3.7,"A",I41&gt;=3.3,"B",I41&gt;=2.8,"C",I41&gt;=2.5,"D",I41&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K41" s="9" t="str" cm="1">
@@ -2278,7 +2277,7 @@
         <v>3.4</v>
       </c>
       <c r="J42" s="9" t="str" cm="1">
-        <f t="array" ref="J42">_xlfn.IFS(I42&gt;=3.7,"A",I42&gt;=3.3,"B",I42&gt;=2.9,"C",I42&gt;=2.6,"D",I42&lt;=2.5,"E")</f>
+        <f t="array" ref="J42">_xlfn.IFS(I42&gt;=3.7,"A",I42&gt;=3.3,"B",I42&gt;=2.8,"C",I42&gt;=2.5,"D",I42&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K42" s="9" t="str" cm="1">
@@ -2319,7 +2318,7 @@
         <v>3.4</v>
       </c>
       <c r="J43" s="9" t="str" cm="1">
-        <f t="array" ref="J43">_xlfn.IFS(I43&gt;=3.7,"A",I43&gt;=3.3,"B",I43&gt;=2.9,"C",I43&gt;=2.6,"D",I43&lt;=2.5,"E")</f>
+        <f t="array" ref="J43">_xlfn.IFS(I43&gt;=3.7,"A",I43&gt;=3.3,"B",I43&gt;=2.8,"C",I43&gt;=2.5,"D",I43&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K43" s="9" t="str" cm="1">
@@ -2360,7 +2359,7 @@
         <v>3.4</v>
       </c>
       <c r="J44" s="9" t="str" cm="1">
-        <f t="array" ref="J44">_xlfn.IFS(I44&gt;=3.7,"A",I44&gt;=3.3,"B",I44&gt;=2.9,"C",I44&gt;=2.6,"D",I44&lt;=2.5,"E")</f>
+        <f t="array" ref="J44">_xlfn.IFS(I44&gt;=3.7,"A",I44&gt;=3.3,"B",I44&gt;=2.8,"C",I44&gt;=2.5,"D",I44&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K44" s="9" t="str" cm="1">
@@ -2401,7 +2400,7 @@
         <v>3.4</v>
       </c>
       <c r="J45" s="9" t="str" cm="1">
-        <f t="array" ref="J45">_xlfn.IFS(I45&gt;=3.7,"A",I45&gt;=3.3,"B",I45&gt;=2.9,"C",I45&gt;=2.6,"D",I45&lt;=2.5,"E")</f>
+        <f t="array" ref="J45">_xlfn.IFS(I45&gt;=3.7,"A",I45&gt;=3.3,"B",I45&gt;=2.8,"C",I45&gt;=2.5,"D",I45&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K45" s="9" t="str" cm="1">
@@ -2442,7 +2441,7 @@
         <v>3.4</v>
       </c>
       <c r="J46" s="9" t="str" cm="1">
-        <f t="array" ref="J46">_xlfn.IFS(I46&gt;=3.7,"A",I46&gt;=3.3,"B",I46&gt;=2.9,"C",I46&gt;=2.6,"D",I46&lt;=2.5,"E")</f>
+        <f t="array" ref="J46">_xlfn.IFS(I46&gt;=3.7,"A",I46&gt;=3.3,"B",I46&gt;=2.8,"C",I46&gt;=2.5,"D",I46&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K46" s="9" t="str" cm="1">
@@ -2483,7 +2482,7 @@
         <v>3.4</v>
       </c>
       <c r="J47" s="9" t="str" cm="1">
-        <f t="array" ref="J47">_xlfn.IFS(I47&gt;=3.7,"A",I47&gt;=3.3,"B",I47&gt;=2.9,"C",I47&gt;=2.6,"D",I47&lt;=2.5,"E")</f>
+        <f t="array" ref="J47">_xlfn.IFS(I47&gt;=3.7,"A",I47&gt;=3.3,"B",I47&gt;=2.8,"C",I47&gt;=2.5,"D",I47&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K47" s="9" t="str" cm="1">
@@ -2524,7 +2523,7 @@
         <v>3.4</v>
       </c>
       <c r="J48" s="9" t="str" cm="1">
-        <f t="array" ref="J48">_xlfn.IFS(I48&gt;=3.7,"A",I48&gt;=3.3,"B",I48&gt;=2.9,"C",I48&gt;=2.6,"D",I48&lt;=2.5,"E")</f>
+        <f t="array" ref="J48">_xlfn.IFS(I48&gt;=3.7,"A",I48&gt;=3.3,"B",I48&gt;=2.8,"C",I48&gt;=2.5,"D",I48&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K48" s="9" t="str" cm="1">
@@ -2565,7 +2564,7 @@
         <v>3.4</v>
       </c>
       <c r="J49" s="9" t="str" cm="1">
-        <f t="array" ref="J49">_xlfn.IFS(I49&gt;=3.7,"A",I49&gt;=3.3,"B",I49&gt;=2.9,"C",I49&gt;=2.6,"D",I49&lt;=2.5,"E")</f>
+        <f t="array" ref="J49">_xlfn.IFS(I49&gt;=3.7,"A",I49&gt;=3.3,"B",I49&gt;=2.8,"C",I49&gt;=2.5,"D",I49&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K49" s="9" t="str" cm="1">
@@ -2606,7 +2605,7 @@
         <v>3.4</v>
       </c>
       <c r="J50" s="9" t="str" cm="1">
-        <f t="array" ref="J50">_xlfn.IFS(I50&gt;=3.7,"A",I50&gt;=3.3,"B",I50&gt;=2.9,"C",I50&gt;=2.6,"D",I50&lt;=2.5,"E")</f>
+        <f t="array" ref="J50">_xlfn.IFS(I50&gt;=3.7,"A",I50&gt;=3.3,"B",I50&gt;=2.8,"C",I50&gt;=2.5,"D",I50&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K50" s="9" t="str" cm="1">
@@ -2647,7 +2646,7 @@
         <v>3.4</v>
       </c>
       <c r="J51" s="9" t="str" cm="1">
-        <f t="array" ref="J51">_xlfn.IFS(I51&gt;=3.7,"A",I51&gt;=3.3,"B",I51&gt;=2.9,"C",I51&gt;=2.6,"D",I51&lt;=2.5,"E")</f>
+        <f t="array" ref="J51">_xlfn.IFS(I51&gt;=3.7,"A",I51&gt;=3.3,"B",I51&gt;=2.8,"C",I51&gt;=2.5,"D",I51&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K51" s="9" t="str" cm="1">
@@ -2688,7 +2687,7 @@
         <v>3.4</v>
       </c>
       <c r="J52" s="9" t="str" cm="1">
-        <f t="array" ref="J52">_xlfn.IFS(I52&gt;=3.7,"A",I52&gt;=3.3,"B",I52&gt;=2.9,"C",I52&gt;=2.6,"D",I52&lt;=2.5,"E")</f>
+        <f t="array" ref="J52">_xlfn.IFS(I52&gt;=3.7,"A",I52&gt;=3.3,"B",I52&gt;=2.8,"C",I52&gt;=2.5,"D",I52&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K52" s="9" t="str" cm="1">
@@ -2729,7 +2728,7 @@
         <v>3.3</v>
       </c>
       <c r="J53" s="9" t="str" cm="1">
-        <f t="array" ref="J53">_xlfn.IFS(I53&gt;=3.7,"A",I53&gt;=3.3,"B",I53&gt;=2.9,"C",I53&gt;=2.6,"D",I53&lt;=2.5,"E")</f>
+        <f t="array" ref="J53">_xlfn.IFS(I53&gt;=3.7,"A",I53&gt;=3.3,"B",I53&gt;=2.8,"C",I53&gt;=2.5,"D",I53&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K53" s="9" t="str" cm="1">
@@ -2770,7 +2769,7 @@
         <v>3.3</v>
       </c>
       <c r="J54" s="9" t="str" cm="1">
-        <f t="array" ref="J54">_xlfn.IFS(I54&gt;=3.7,"A",I54&gt;=3.3,"B",I54&gt;=2.9,"C",I54&gt;=2.6,"D",I54&lt;=2.5,"E")</f>
+        <f t="array" ref="J54">_xlfn.IFS(I54&gt;=3.7,"A",I54&gt;=3.3,"B",I54&gt;=2.8,"C",I54&gt;=2.5,"D",I54&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K54" s="9" t="str" cm="1">
@@ -2811,7 +2810,7 @@
         <v>3.3</v>
       </c>
       <c r="J55" s="9" t="str" cm="1">
-        <f t="array" ref="J55">_xlfn.IFS(I55&gt;=3.7,"A",I55&gt;=3.3,"B",I55&gt;=2.9,"C",I55&gt;=2.6,"D",I55&lt;=2.5,"E")</f>
+        <f t="array" ref="J55">_xlfn.IFS(I55&gt;=3.7,"A",I55&gt;=3.3,"B",I55&gt;=2.8,"C",I55&gt;=2.5,"D",I55&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K55" s="9" t="str" cm="1">
@@ -2852,7 +2851,7 @@
         <v>3.3</v>
       </c>
       <c r="J56" s="9" t="str" cm="1">
-        <f t="array" ref="J56">_xlfn.IFS(I56&gt;=3.7,"A",I56&gt;=3.3,"B",I56&gt;=2.9,"C",I56&gt;=2.6,"D",I56&lt;=2.5,"E")</f>
+        <f t="array" ref="J56">_xlfn.IFS(I56&gt;=3.7,"A",I56&gt;=3.3,"B",I56&gt;=2.8,"C",I56&gt;=2.5,"D",I56&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K56" s="9" t="str" cm="1">
@@ -2893,7 +2892,7 @@
         <v>3.3</v>
       </c>
       <c r="J57" s="9" t="str" cm="1">
-        <f t="array" ref="J57">_xlfn.IFS(I57&gt;=3.7,"A",I57&gt;=3.3,"B",I57&gt;=2.9,"C",I57&gt;=2.6,"D",I57&lt;=2.5,"E")</f>
+        <f t="array" ref="J57">_xlfn.IFS(I57&gt;=3.7,"A",I57&gt;=3.3,"B",I57&gt;=2.8,"C",I57&gt;=2.5,"D",I57&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K57" s="9" t="str" cm="1">
@@ -2934,7 +2933,7 @@
         <v>3.3</v>
       </c>
       <c r="J58" s="9" t="str" cm="1">
-        <f t="array" ref="J58">_xlfn.IFS(I58&gt;=3.7,"A",I58&gt;=3.3,"B",I58&gt;=2.9,"C",I58&gt;=2.6,"D",I58&lt;=2.5,"E")</f>
+        <f t="array" ref="J58">_xlfn.IFS(I58&gt;=3.7,"A",I58&gt;=3.3,"B",I58&gt;=2.8,"C",I58&gt;=2.5,"D",I58&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K58" s="9" t="str" cm="1">
@@ -2975,7 +2974,7 @@
         <v>3.3</v>
       </c>
       <c r="J59" s="9" t="str" cm="1">
-        <f t="array" ref="J59">_xlfn.IFS(I59&gt;=3.7,"A",I59&gt;=3.3,"B",I59&gt;=2.9,"C",I59&gt;=2.6,"D",I59&lt;=2.5,"E")</f>
+        <f t="array" ref="J59">_xlfn.IFS(I59&gt;=3.7,"A",I59&gt;=3.3,"B",I59&gt;=2.8,"C",I59&gt;=2.5,"D",I59&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K59" s="9" t="str" cm="1">
@@ -3016,7 +3015,7 @@
         <v>3.3</v>
       </c>
       <c r="J60" s="9" t="str" cm="1">
-        <f t="array" ref="J60">_xlfn.IFS(I60&gt;=3.7,"A",I60&gt;=3.3,"B",I60&gt;=2.9,"C",I60&gt;=2.6,"D",I60&lt;=2.5,"E")</f>
+        <f t="array" ref="J60">_xlfn.IFS(I60&gt;=3.7,"A",I60&gt;=3.3,"B",I60&gt;=2.8,"C",I60&gt;=2.5,"D",I60&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K60" s="9" t="str" cm="1">
@@ -3057,7 +3056,7 @@
         <v>3.3</v>
       </c>
       <c r="J61" s="9" t="str" cm="1">
-        <f t="array" ref="J61">_xlfn.IFS(I61&gt;=3.7,"A",I61&gt;=3.3,"B",I61&gt;=2.9,"C",I61&gt;=2.6,"D",I61&lt;=2.5,"E")</f>
+        <f t="array" ref="J61">_xlfn.IFS(I61&gt;=3.7,"A",I61&gt;=3.3,"B",I61&gt;=2.8,"C",I61&gt;=2.5,"D",I61&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K61" s="9" t="str" cm="1">
@@ -3098,7 +3097,7 @@
         <v>3.3</v>
       </c>
       <c r="J62" s="9" t="str" cm="1">
-        <f t="array" ref="J62">_xlfn.IFS(I62&gt;=3.7,"A",I62&gt;=3.3,"B",I62&gt;=2.9,"C",I62&gt;=2.6,"D",I62&lt;=2.5,"E")</f>
+        <f t="array" ref="J62">_xlfn.IFS(I62&gt;=3.7,"A",I62&gt;=3.3,"B",I62&gt;=2.8,"C",I62&gt;=2.5,"D",I62&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K62" s="9" t="str" cm="1">
@@ -3139,7 +3138,7 @@
         <v>3.3</v>
       </c>
       <c r="J63" s="9" t="str" cm="1">
-        <f t="array" ref="J63">_xlfn.IFS(I63&gt;=3.7,"A",I63&gt;=3.3,"B",I63&gt;=2.9,"C",I63&gt;=2.6,"D",I63&lt;=2.5,"E")</f>
+        <f t="array" ref="J63">_xlfn.IFS(I63&gt;=3.7,"A",I63&gt;=3.3,"B",I63&gt;=2.8,"C",I63&gt;=2.5,"D",I63&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K63" s="9" t="str" cm="1">
@@ -3180,7 +3179,7 @@
         <v>3.3</v>
       </c>
       <c r="J64" s="9" t="str" cm="1">
-        <f t="array" ref="J64">_xlfn.IFS(I64&gt;=3.7,"A",I64&gt;=3.3,"B",I64&gt;=2.9,"C",I64&gt;=2.6,"D",I64&lt;=2.5,"E")</f>
+        <f t="array" ref="J64">_xlfn.IFS(I64&gt;=3.7,"A",I64&gt;=3.3,"B",I64&gt;=2.8,"C",I64&gt;=2.5,"D",I64&lt;=2.4,"E")</f>
         <v>B</v>
       </c>
       <c r="K64" s="9" t="str" cm="1">
@@ -3221,7 +3220,7 @@
         <v>3.2</v>
       </c>
       <c r="J65" s="9" t="str" cm="1">
-        <f t="array" ref="J65">_xlfn.IFS(I65&gt;=3.7,"A",I65&gt;=3.3,"B",I65&gt;=2.9,"C",I65&gt;=2.6,"D",I65&lt;=2.5,"E")</f>
+        <f t="array" ref="J65">_xlfn.IFS(I65&gt;=3.7,"A",I65&gt;=3.3,"B",I65&gt;=2.8,"C",I65&gt;=2.5,"D",I65&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K65" s="9" t="str" cm="1">
@@ -3262,7 +3261,7 @@
         <v>3.2</v>
       </c>
       <c r="J66" s="9" t="str" cm="1">
-        <f t="array" ref="J66">_xlfn.IFS(I66&gt;=3.7,"A",I66&gt;=3.3,"B",I66&gt;=2.9,"C",I66&gt;=2.6,"D",I66&lt;=2.5,"E")</f>
+        <f t="array" ref="J66">_xlfn.IFS(I66&gt;=3.7,"A",I66&gt;=3.3,"B",I66&gt;=2.8,"C",I66&gt;=2.5,"D",I66&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K66" s="9" t="str" cm="1">
@@ -3303,7 +3302,7 @@
         <v>3.2</v>
       </c>
       <c r="J67" s="9" t="str" cm="1">
-        <f t="array" ref="J67">_xlfn.IFS(I67&gt;=3.7,"A",I67&gt;=3.3,"B",I67&gt;=2.9,"C",I67&gt;=2.6,"D",I67&lt;=2.5,"E")</f>
+        <f t="array" ref="J67">_xlfn.IFS(I67&gt;=3.7,"A",I67&gt;=3.3,"B",I67&gt;=2.8,"C",I67&gt;=2.5,"D",I67&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K67" s="9" t="str" cm="1">
@@ -3344,7 +3343,7 @@
         <v>3.2</v>
       </c>
       <c r="J68" s="9" t="str" cm="1">
-        <f t="array" ref="J68">_xlfn.IFS(I68&gt;=3.7,"A",I68&gt;=3.3,"B",I68&gt;=2.9,"C",I68&gt;=2.6,"D",I68&lt;=2.5,"E")</f>
+        <f t="array" ref="J68">_xlfn.IFS(I68&gt;=3.7,"A",I68&gt;=3.3,"B",I68&gt;=2.8,"C",I68&gt;=2.5,"D",I68&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K68" s="9" t="str" cm="1">
@@ -3385,7 +3384,7 @@
         <v>3.2</v>
       </c>
       <c r="J69" s="9" t="str" cm="1">
-        <f t="array" ref="J69">_xlfn.IFS(I69&gt;=3.7,"A",I69&gt;=3.3,"B",I69&gt;=2.9,"C",I69&gt;=2.6,"D",I69&lt;=2.5,"E")</f>
+        <f t="array" ref="J69">_xlfn.IFS(I69&gt;=3.7,"A",I69&gt;=3.3,"B",I69&gt;=2.8,"C",I69&gt;=2.5,"D",I69&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K69" s="9" t="str" cm="1">
@@ -3426,7 +3425,7 @@
         <v>3.2</v>
       </c>
       <c r="J70" s="9" t="str" cm="1">
-        <f t="array" ref="J70">_xlfn.IFS(I70&gt;=3.7,"A",I70&gt;=3.3,"B",I70&gt;=2.9,"C",I70&gt;=2.6,"D",I70&lt;=2.5,"E")</f>
+        <f t="array" ref="J70">_xlfn.IFS(I70&gt;=3.7,"A",I70&gt;=3.3,"B",I70&gt;=2.8,"C",I70&gt;=2.5,"D",I70&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K70" s="9" t="str" cm="1">
@@ -3467,7 +3466,7 @@
         <v>3.2</v>
       </c>
       <c r="J71" s="9" t="str" cm="1">
-        <f t="array" ref="J71">_xlfn.IFS(I71&gt;=3.7,"A",I71&gt;=3.3,"B",I71&gt;=2.9,"C",I71&gt;=2.6,"D",I71&lt;=2.5,"E")</f>
+        <f t="array" ref="J71">_xlfn.IFS(I71&gt;=3.7,"A",I71&gt;=3.3,"B",I71&gt;=2.8,"C",I71&gt;=2.5,"D",I71&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K71" s="9" t="str" cm="1">
@@ -3508,7 +3507,7 @@
         <v>3.2</v>
       </c>
       <c r="J72" s="9" t="str" cm="1">
-        <f t="array" ref="J72">_xlfn.IFS(I72&gt;=3.7,"A",I72&gt;=3.3,"B",I72&gt;=2.9,"C",I72&gt;=2.6,"D",I72&lt;=2.5,"E")</f>
+        <f t="array" ref="J72">_xlfn.IFS(I72&gt;=3.7,"A",I72&gt;=3.3,"B",I72&gt;=2.8,"C",I72&gt;=2.5,"D",I72&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K72" s="9" t="str" cm="1">
@@ -3549,7 +3548,7 @@
         <v>3.2</v>
       </c>
       <c r="J73" s="9" t="str" cm="1">
-        <f t="array" ref="J73">_xlfn.IFS(I73&gt;=3.7,"A",I73&gt;=3.3,"B",I73&gt;=2.9,"C",I73&gt;=2.6,"D",I73&lt;=2.5,"E")</f>
+        <f t="array" ref="J73">_xlfn.IFS(I73&gt;=3.7,"A",I73&gt;=3.3,"B",I73&gt;=2.8,"C",I73&gt;=2.5,"D",I73&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K73" s="9" t="str" cm="1">
@@ -3590,7 +3589,7 @@
         <v>3.2</v>
       </c>
       <c r="J74" s="9" t="str" cm="1">
-        <f t="array" ref="J74">_xlfn.IFS(I74&gt;=3.7,"A",I74&gt;=3.3,"B",I74&gt;=2.9,"C",I74&gt;=2.6,"D",I74&lt;=2.5,"E")</f>
+        <f t="array" ref="J74">_xlfn.IFS(I74&gt;=3.7,"A",I74&gt;=3.3,"B",I74&gt;=2.8,"C",I74&gt;=2.5,"D",I74&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K74" s="9" t="str" cm="1">
@@ -3631,7 +3630,7 @@
         <v>3.2</v>
       </c>
       <c r="J75" s="9" t="str" cm="1">
-        <f t="array" ref="J75">_xlfn.IFS(I75&gt;=3.7,"A",I75&gt;=3.3,"B",I75&gt;=2.9,"C",I75&gt;=2.6,"D",I75&lt;=2.5,"E")</f>
+        <f t="array" ref="J75">_xlfn.IFS(I75&gt;=3.7,"A",I75&gt;=3.3,"B",I75&gt;=2.8,"C",I75&gt;=2.5,"D",I75&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K75" s="9" t="str" cm="1">
@@ -3672,7 +3671,7 @@
         <v>3.2</v>
       </c>
       <c r="J76" s="9" t="str" cm="1">
-        <f t="array" ref="J76">_xlfn.IFS(I76&gt;=3.7,"A",I76&gt;=3.3,"B",I76&gt;=2.9,"C",I76&gt;=2.6,"D",I76&lt;=2.5,"E")</f>
+        <f t="array" ref="J76">_xlfn.IFS(I76&gt;=3.7,"A",I76&gt;=3.3,"B",I76&gt;=2.8,"C",I76&gt;=2.5,"D",I76&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K76" s="9" t="str" cm="1">
@@ -3713,7 +3712,7 @@
         <v>3.2</v>
       </c>
       <c r="J77" s="9" t="str" cm="1">
-        <f t="array" ref="J77">_xlfn.IFS(I77&gt;=3.7,"A",I77&gt;=3.3,"B",I77&gt;=2.9,"C",I77&gt;=2.6,"D",I77&lt;=2.5,"E")</f>
+        <f t="array" ref="J77">_xlfn.IFS(I77&gt;=3.7,"A",I77&gt;=3.3,"B",I77&gt;=2.8,"C",I77&gt;=2.5,"D",I77&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K77" s="9" t="str" cm="1">
@@ -3754,7 +3753,7 @@
         <v>3.2</v>
       </c>
       <c r="J78" s="9" t="str" cm="1">
-        <f t="array" ref="J78">_xlfn.IFS(I78&gt;=3.7,"A",I78&gt;=3.3,"B",I78&gt;=2.9,"C",I78&gt;=2.6,"D",I78&lt;=2.5,"E")</f>
+        <f t="array" ref="J78">_xlfn.IFS(I78&gt;=3.7,"A",I78&gt;=3.3,"B",I78&gt;=2.8,"C",I78&gt;=2.5,"D",I78&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K78" s="9" t="str" cm="1">
@@ -3795,7 +3794,7 @@
         <v>3.2</v>
       </c>
       <c r="J79" s="9" t="str" cm="1">
-        <f t="array" ref="J79">_xlfn.IFS(I79&gt;=3.7,"A",I79&gt;=3.3,"B",I79&gt;=2.9,"C",I79&gt;=2.6,"D",I79&lt;=2.5,"E")</f>
+        <f t="array" ref="J79">_xlfn.IFS(I79&gt;=3.7,"A",I79&gt;=3.3,"B",I79&gt;=2.8,"C",I79&gt;=2.5,"D",I79&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K79" s="9" t="str" cm="1">
@@ -3836,7 +3835,7 @@
         <v>3.2</v>
       </c>
       <c r="J80" s="9" t="str" cm="1">
-        <f t="array" ref="J80">_xlfn.IFS(I80&gt;=3.7,"A",I80&gt;=3.3,"B",I80&gt;=2.9,"C",I80&gt;=2.6,"D",I80&lt;=2.5,"E")</f>
+        <f t="array" ref="J80">_xlfn.IFS(I80&gt;=3.7,"A",I80&gt;=3.3,"B",I80&gt;=2.8,"C",I80&gt;=2.5,"D",I80&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K80" s="9" t="str" cm="1">
@@ -3877,7 +3876,7 @@
         <v>3.2</v>
       </c>
       <c r="J81" s="9" t="str" cm="1">
-        <f t="array" ref="J81">_xlfn.IFS(I81&gt;=3.7,"A",I81&gt;=3.3,"B",I81&gt;=2.9,"C",I81&gt;=2.6,"D",I81&lt;=2.5,"E")</f>
+        <f t="array" ref="J81">_xlfn.IFS(I81&gt;=3.7,"A",I81&gt;=3.3,"B",I81&gt;=2.8,"C",I81&gt;=2.5,"D",I81&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K81" s="9" t="str" cm="1">
@@ -3918,7 +3917,7 @@
         <v>3.2</v>
       </c>
       <c r="J82" s="9" t="str" cm="1">
-        <f t="array" ref="J82">_xlfn.IFS(I82&gt;=3.7,"A",I82&gt;=3.3,"B",I82&gt;=2.9,"C",I82&gt;=2.6,"D",I82&lt;=2.5,"E")</f>
+        <f t="array" ref="J82">_xlfn.IFS(I82&gt;=3.7,"A",I82&gt;=3.3,"B",I82&gt;=2.8,"C",I82&gt;=2.5,"D",I82&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K82" s="9" t="str" cm="1">
@@ -3959,7 +3958,7 @@
         <v>3.2</v>
       </c>
       <c r="J83" s="9" t="str" cm="1">
-        <f t="array" ref="J83">_xlfn.IFS(I83&gt;=3.7,"A",I83&gt;=3.3,"B",I83&gt;=2.9,"C",I83&gt;=2.6,"D",I83&lt;=2.5,"E")</f>
+        <f t="array" ref="J83">_xlfn.IFS(I83&gt;=3.7,"A",I83&gt;=3.3,"B",I83&gt;=2.8,"C",I83&gt;=2.5,"D",I83&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K83" s="9" t="str" cm="1">
@@ -4000,7 +3999,7 @@
         <v>3.2</v>
       </c>
       <c r="J84" s="9" t="str" cm="1">
-        <f t="array" ref="J84">_xlfn.IFS(I84&gt;=3.7,"A",I84&gt;=3.3,"B",I84&gt;=2.9,"C",I84&gt;=2.6,"D",I84&lt;=2.5,"E")</f>
+        <f t="array" ref="J84">_xlfn.IFS(I84&gt;=3.7,"A",I84&gt;=3.3,"B",I84&gt;=2.8,"C",I84&gt;=2.5,"D",I84&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K84" s="9" t="str" cm="1">
@@ -4041,7 +4040,7 @@
         <v>3.1</v>
       </c>
       <c r="J85" s="9" t="str" cm="1">
-        <f t="array" ref="J85">_xlfn.IFS(I85&gt;=3.7,"A",I85&gt;=3.3,"B",I85&gt;=2.9,"C",I85&gt;=2.6,"D",I85&lt;=2.5,"E")</f>
+        <f t="array" ref="J85">_xlfn.IFS(I85&gt;=3.7,"A",I85&gt;=3.3,"B",I85&gt;=2.8,"C",I85&gt;=2.5,"D",I85&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K85" s="9" t="str" cm="1">
@@ -4082,7 +4081,7 @@
         <v>3.1</v>
       </c>
       <c r="J86" s="9" t="str" cm="1">
-        <f t="array" ref="J86">_xlfn.IFS(I86&gt;=3.7,"A",I86&gt;=3.3,"B",I86&gt;=2.9,"C",I86&gt;=2.6,"D",I86&lt;=2.5,"E")</f>
+        <f t="array" ref="J86">_xlfn.IFS(I86&gt;=3.7,"A",I86&gt;=3.3,"B",I86&gt;=2.8,"C",I86&gt;=2.5,"D",I86&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K86" s="9" t="str" cm="1">
@@ -4123,7 +4122,7 @@
         <v>3.1</v>
       </c>
       <c r="J87" s="9" t="str" cm="1">
-        <f t="array" ref="J87">_xlfn.IFS(I87&gt;=3.7,"A",I87&gt;=3.3,"B",I87&gt;=2.9,"C",I87&gt;=2.6,"D",I87&lt;=2.5,"E")</f>
+        <f t="array" ref="J87">_xlfn.IFS(I87&gt;=3.7,"A",I87&gt;=3.3,"B",I87&gt;=2.8,"C",I87&gt;=2.5,"D",I87&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K87" s="9" t="str" cm="1">
@@ -4164,7 +4163,7 @@
         <v>3.1</v>
       </c>
       <c r="J88" s="9" t="str" cm="1">
-        <f t="array" ref="J88">_xlfn.IFS(I88&gt;=3.7,"A",I88&gt;=3.3,"B",I88&gt;=2.9,"C",I88&gt;=2.6,"D",I88&lt;=2.5,"E")</f>
+        <f t="array" ref="J88">_xlfn.IFS(I88&gt;=3.7,"A",I88&gt;=3.3,"B",I88&gt;=2.8,"C",I88&gt;=2.5,"D",I88&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K88" s="9" t="str" cm="1">
@@ -4205,7 +4204,7 @@
         <v>3.1</v>
       </c>
       <c r="J89" s="9" t="str" cm="1">
-        <f t="array" ref="J89">_xlfn.IFS(I89&gt;=3.7,"A",I89&gt;=3.3,"B",I89&gt;=2.9,"C",I89&gt;=2.6,"D",I89&lt;=2.5,"E")</f>
+        <f t="array" ref="J89">_xlfn.IFS(I89&gt;=3.7,"A",I89&gt;=3.3,"B",I89&gt;=2.8,"C",I89&gt;=2.5,"D",I89&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K89" s="9" t="str" cm="1">
@@ -4246,7 +4245,7 @@
         <v>3.1</v>
       </c>
       <c r="J90" s="9" t="str" cm="1">
-        <f t="array" ref="J90">_xlfn.IFS(I90&gt;=3.7,"A",I90&gt;=3.3,"B",I90&gt;=2.9,"C",I90&gt;=2.6,"D",I90&lt;=2.5,"E")</f>
+        <f t="array" ref="J90">_xlfn.IFS(I90&gt;=3.7,"A",I90&gt;=3.3,"B",I90&gt;=2.8,"C",I90&gt;=2.5,"D",I90&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K90" s="9" t="str" cm="1">
@@ -4287,7 +4286,7 @@
         <v>3.1</v>
       </c>
       <c r="J91" s="9" t="str" cm="1">
-        <f t="array" ref="J91">_xlfn.IFS(I91&gt;=3.7,"A",I91&gt;=3.3,"B",I91&gt;=2.9,"C",I91&gt;=2.6,"D",I91&lt;=2.5,"E")</f>
+        <f t="array" ref="J91">_xlfn.IFS(I91&gt;=3.7,"A",I91&gt;=3.3,"B",I91&gt;=2.8,"C",I91&gt;=2.5,"D",I91&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K91" s="9" t="str" cm="1">
@@ -4328,7 +4327,7 @@
         <v>3.1</v>
       </c>
       <c r="J92" s="9" t="str" cm="1">
-        <f t="array" ref="J92">_xlfn.IFS(I92&gt;=3.7,"A",I92&gt;=3.3,"B",I92&gt;=2.9,"C",I92&gt;=2.6,"D",I92&lt;=2.5,"E")</f>
+        <f t="array" ref="J92">_xlfn.IFS(I92&gt;=3.7,"A",I92&gt;=3.3,"B",I92&gt;=2.8,"C",I92&gt;=2.5,"D",I92&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K92" s="9" t="str" cm="1">
@@ -4369,7 +4368,7 @@
         <v>3.1</v>
       </c>
       <c r="J93" s="9" t="str" cm="1">
-        <f t="array" ref="J93">_xlfn.IFS(I93&gt;=3.7,"A",I93&gt;=3.3,"B",I93&gt;=2.9,"C",I93&gt;=2.6,"D",I93&lt;=2.5,"E")</f>
+        <f t="array" ref="J93">_xlfn.IFS(I93&gt;=3.7,"A",I93&gt;=3.3,"B",I93&gt;=2.8,"C",I93&gt;=2.5,"D",I93&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K93" s="9" t="str" cm="1">
@@ -4410,7 +4409,7 @@
         <v>3.1</v>
       </c>
       <c r="J94" s="9" t="str" cm="1">
-        <f t="array" ref="J94">_xlfn.IFS(I94&gt;=3.7,"A",I94&gt;=3.3,"B",I94&gt;=2.9,"C",I94&gt;=2.6,"D",I94&lt;=2.5,"E")</f>
+        <f t="array" ref="J94">_xlfn.IFS(I94&gt;=3.7,"A",I94&gt;=3.3,"B",I94&gt;=2.8,"C",I94&gt;=2.5,"D",I94&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K94" s="9" t="str" cm="1">
@@ -4451,7 +4450,7 @@
         <v>3.1</v>
       </c>
       <c r="J95" s="9" t="str" cm="1">
-        <f t="array" ref="J95">_xlfn.IFS(I95&gt;=3.7,"A",I95&gt;=3.3,"B",I95&gt;=2.9,"C",I95&gt;=2.6,"D",I95&lt;=2.5,"E")</f>
+        <f t="array" ref="J95">_xlfn.IFS(I95&gt;=3.7,"A",I95&gt;=3.3,"B",I95&gt;=2.8,"C",I95&gt;=2.5,"D",I95&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K95" s="9" t="str" cm="1">
@@ -4492,7 +4491,7 @@
         <v>3.1</v>
       </c>
       <c r="J96" s="9" t="str" cm="1">
-        <f t="array" ref="J96">_xlfn.IFS(I96&gt;=3.7,"A",I96&gt;=3.3,"B",I96&gt;=2.9,"C",I96&gt;=2.6,"D",I96&lt;=2.5,"E")</f>
+        <f t="array" ref="J96">_xlfn.IFS(I96&gt;=3.7,"A",I96&gt;=3.3,"B",I96&gt;=2.8,"C",I96&gt;=2.5,"D",I96&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K96" s="9" t="str" cm="1">
@@ -4533,7 +4532,7 @@
         <v>3.1</v>
       </c>
       <c r="J97" s="9" t="str" cm="1">
-        <f t="array" ref="J97">_xlfn.IFS(I97&gt;=3.7,"A",I97&gt;=3.3,"B",I97&gt;=2.9,"C",I97&gt;=2.6,"D",I97&lt;=2.5,"E")</f>
+        <f t="array" ref="J97">_xlfn.IFS(I97&gt;=3.7,"A",I97&gt;=3.3,"B",I97&gt;=2.8,"C",I97&gt;=2.5,"D",I97&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K97" s="9" t="str" cm="1">
@@ -4574,7 +4573,7 @@
         <v>3.1</v>
       </c>
       <c r="J98" s="9" t="str" cm="1">
-        <f t="array" ref="J98">_xlfn.IFS(I98&gt;=3.7,"A",I98&gt;=3.3,"B",I98&gt;=2.9,"C",I98&gt;=2.6,"D",I98&lt;=2.5,"E")</f>
+        <f t="array" ref="J98">_xlfn.IFS(I98&gt;=3.7,"A",I98&gt;=3.3,"B",I98&gt;=2.8,"C",I98&gt;=2.5,"D",I98&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K98" s="9" t="str" cm="1">
@@ -4615,7 +4614,7 @@
         <v>3.1</v>
       </c>
       <c r="J99" s="9" t="str" cm="1">
-        <f t="array" ref="J99">_xlfn.IFS(I99&gt;=3.7,"A",I99&gt;=3.3,"B",I99&gt;=2.9,"C",I99&gt;=2.6,"D",I99&lt;=2.5,"E")</f>
+        <f t="array" ref="J99">_xlfn.IFS(I99&gt;=3.7,"A",I99&gt;=3.3,"B",I99&gt;=2.8,"C",I99&gt;=2.5,"D",I99&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K99" s="9" t="str" cm="1">
@@ -4656,7 +4655,7 @@
         <v>3</v>
       </c>
       <c r="J100" s="9" t="str" cm="1">
-        <f t="array" ref="J100">_xlfn.IFS(I100&gt;=3.7,"A",I100&gt;=3.3,"B",I100&gt;=2.9,"C",I100&gt;=2.6,"D",I100&lt;=2.5,"E")</f>
+        <f t="array" ref="J100">_xlfn.IFS(I100&gt;=3.7,"A",I100&gt;=3.3,"B",I100&gt;=2.8,"C",I100&gt;=2.5,"D",I100&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K100" s="9" t="str" cm="1">
@@ -4697,7 +4696,7 @@
         <v>3</v>
       </c>
       <c r="J101" s="9" t="str" cm="1">
-        <f t="array" ref="J101">_xlfn.IFS(I101&gt;=3.7,"A",I101&gt;=3.3,"B",I101&gt;=2.9,"C",I101&gt;=2.6,"D",I101&lt;=2.5,"E")</f>
+        <f t="array" ref="J101">_xlfn.IFS(I101&gt;=3.7,"A",I101&gt;=3.3,"B",I101&gt;=2.8,"C",I101&gt;=2.5,"D",I101&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K101" s="9" t="str" cm="1">
@@ -4738,7 +4737,7 @@
         <v>3</v>
       </c>
       <c r="J102" s="9" t="str" cm="1">
-        <f t="array" ref="J102">_xlfn.IFS(I102&gt;=3.7,"A",I102&gt;=3.3,"B",I102&gt;=2.9,"C",I102&gt;=2.6,"D",I102&lt;=2.5,"E")</f>
+        <f t="array" ref="J102">_xlfn.IFS(I102&gt;=3.7,"A",I102&gt;=3.3,"B",I102&gt;=2.8,"C",I102&gt;=2.5,"D",I102&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K102" s="9" t="str" cm="1">
@@ -4779,7 +4778,7 @@
         <v>3</v>
       </c>
       <c r="J103" s="9" t="str" cm="1">
-        <f t="array" ref="J103">_xlfn.IFS(I103&gt;=3.7,"A",I103&gt;=3.3,"B",I103&gt;=2.9,"C",I103&gt;=2.6,"D",I103&lt;=2.5,"E")</f>
+        <f t="array" ref="J103">_xlfn.IFS(I103&gt;=3.7,"A",I103&gt;=3.3,"B",I103&gt;=2.8,"C",I103&gt;=2.5,"D",I103&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K103" s="9" t="str" cm="1">
@@ -4820,7 +4819,7 @@
         <v>3</v>
       </c>
       <c r="J104" s="9" t="str" cm="1">
-        <f t="array" ref="J104">_xlfn.IFS(I104&gt;=3.7,"A",I104&gt;=3.3,"B",I104&gt;=2.9,"C",I104&gt;=2.6,"D",I104&lt;=2.5,"E")</f>
+        <f t="array" ref="J104">_xlfn.IFS(I104&gt;=3.7,"A",I104&gt;=3.3,"B",I104&gt;=2.8,"C",I104&gt;=2.5,"D",I104&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K104" s="9" t="str" cm="1">
@@ -4861,7 +4860,7 @@
         <v>3</v>
       </c>
       <c r="J105" s="9" t="str" cm="1">
-        <f t="array" ref="J105">_xlfn.IFS(I105&gt;=3.7,"A",I105&gt;=3.3,"B",I105&gt;=2.9,"C",I105&gt;=2.6,"D",I105&lt;=2.5,"E")</f>
+        <f t="array" ref="J105">_xlfn.IFS(I105&gt;=3.7,"A",I105&gt;=3.3,"B",I105&gt;=2.8,"C",I105&gt;=2.5,"D",I105&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K105" s="9" t="str" cm="1">
@@ -4902,7 +4901,7 @@
         <v>3</v>
       </c>
       <c r="J106" s="9" t="str" cm="1">
-        <f t="array" ref="J106">_xlfn.IFS(I106&gt;=3.7,"A",I106&gt;=3.3,"B",I106&gt;=2.9,"C",I106&gt;=2.6,"D",I106&lt;=2.5,"E")</f>
+        <f t="array" ref="J106">_xlfn.IFS(I106&gt;=3.7,"A",I106&gt;=3.3,"B",I106&gt;=2.8,"C",I106&gt;=2.5,"D",I106&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K106" s="9" t="str" cm="1">
@@ -4943,7 +4942,7 @@
         <v>3</v>
       </c>
       <c r="J107" s="9" t="str" cm="1">
-        <f t="array" ref="J107">_xlfn.IFS(I107&gt;=3.7,"A",I107&gt;=3.3,"B",I107&gt;=2.9,"C",I107&gt;=2.6,"D",I107&lt;=2.5,"E")</f>
+        <f t="array" ref="J107">_xlfn.IFS(I107&gt;=3.7,"A",I107&gt;=3.3,"B",I107&gt;=2.8,"C",I107&gt;=2.5,"D",I107&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K107" s="9" t="str" cm="1">
@@ -4984,7 +4983,7 @@
         <v>3</v>
       </c>
       <c r="J108" s="9" t="str" cm="1">
-        <f t="array" ref="J108">_xlfn.IFS(I108&gt;=3.7,"A",I108&gt;=3.3,"B",I108&gt;=2.9,"C",I108&gt;=2.6,"D",I108&lt;=2.5,"E")</f>
+        <f t="array" ref="J108">_xlfn.IFS(I108&gt;=3.7,"A",I108&gt;=3.3,"B",I108&gt;=2.8,"C",I108&gt;=2.5,"D",I108&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K108" s="9" t="str" cm="1">
@@ -5025,7 +5024,7 @@
         <v>3</v>
       </c>
       <c r="J109" s="9" t="str" cm="1">
-        <f t="array" ref="J109">_xlfn.IFS(I109&gt;=3.7,"A",I109&gt;=3.3,"B",I109&gt;=2.9,"C",I109&gt;=2.6,"D",I109&lt;=2.5,"E")</f>
+        <f t="array" ref="J109">_xlfn.IFS(I109&gt;=3.7,"A",I109&gt;=3.3,"B",I109&gt;=2.8,"C",I109&gt;=2.5,"D",I109&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K109" s="9" t="str" cm="1">
@@ -5066,7 +5065,7 @@
         <v>3</v>
       </c>
       <c r="J110" s="9" t="str" cm="1">
-        <f t="array" ref="J110">_xlfn.IFS(I110&gt;=3.7,"A",I110&gt;=3.3,"B",I110&gt;=2.9,"C",I110&gt;=2.6,"D",I110&lt;=2.5,"E")</f>
+        <f t="array" ref="J110">_xlfn.IFS(I110&gt;=3.7,"A",I110&gt;=3.3,"B",I110&gt;=2.8,"C",I110&gt;=2.5,"D",I110&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K110" s="9" t="str" cm="1">
@@ -5107,7 +5106,7 @@
         <v>3</v>
       </c>
       <c r="J111" s="9" t="str" cm="1">
-        <f t="array" ref="J111">_xlfn.IFS(I111&gt;=3.7,"A",I111&gt;=3.3,"B",I111&gt;=2.9,"C",I111&gt;=2.6,"D",I111&lt;=2.5,"E")</f>
+        <f t="array" ref="J111">_xlfn.IFS(I111&gt;=3.7,"A",I111&gt;=3.3,"B",I111&gt;=2.8,"C",I111&gt;=2.5,"D",I111&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K111" s="9" t="str" cm="1">
@@ -5148,7 +5147,7 @@
         <v>3</v>
       </c>
       <c r="J112" s="9" t="str" cm="1">
-        <f t="array" ref="J112">_xlfn.IFS(I112&gt;=3.7,"A",I112&gt;=3.3,"B",I112&gt;=2.9,"C",I112&gt;=2.6,"D",I112&lt;=2.5,"E")</f>
+        <f t="array" ref="J112">_xlfn.IFS(I112&gt;=3.7,"A",I112&gt;=3.3,"B",I112&gt;=2.8,"C",I112&gt;=2.5,"D",I112&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K112" s="9" t="str" cm="1">
@@ -5189,7 +5188,7 @@
         <v>3</v>
       </c>
       <c r="J113" s="9" t="str" cm="1">
-        <f t="array" ref="J113">_xlfn.IFS(I113&gt;=3.7,"A",I113&gt;=3.3,"B",I113&gt;=2.9,"C",I113&gt;=2.6,"D",I113&lt;=2.5,"E")</f>
+        <f t="array" ref="J113">_xlfn.IFS(I113&gt;=3.7,"A",I113&gt;=3.3,"B",I113&gt;=2.8,"C",I113&gt;=2.5,"D",I113&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K113" s="9" t="str" cm="1">
@@ -5230,7 +5229,7 @@
         <v>3</v>
       </c>
       <c r="J114" s="9" t="str" cm="1">
-        <f t="array" ref="J114">_xlfn.IFS(I114&gt;=3.7,"A",I114&gt;=3.3,"B",I114&gt;=2.9,"C",I114&gt;=2.6,"D",I114&lt;=2.5,"E")</f>
+        <f t="array" ref="J114">_xlfn.IFS(I114&gt;=3.7,"A",I114&gt;=3.3,"B",I114&gt;=2.8,"C",I114&gt;=2.5,"D",I114&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K114" s="9" t="str" cm="1">
@@ -5271,7 +5270,7 @@
         <v>3</v>
       </c>
       <c r="J115" s="9" t="str" cm="1">
-        <f t="array" ref="J115">_xlfn.IFS(I115&gt;=3.7,"A",I115&gt;=3.3,"B",I115&gt;=2.9,"C",I115&gt;=2.6,"D",I115&lt;=2.5,"E")</f>
+        <f t="array" ref="J115">_xlfn.IFS(I115&gt;=3.7,"A",I115&gt;=3.3,"B",I115&gt;=2.8,"C",I115&gt;=2.5,"D",I115&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K115" s="9" t="str" cm="1">
@@ -5312,7 +5311,7 @@
         <v>3</v>
       </c>
       <c r="J116" s="9" t="str" cm="1">
-        <f t="array" ref="J116">_xlfn.IFS(I116&gt;=3.7,"A",I116&gt;=3.3,"B",I116&gt;=2.9,"C",I116&gt;=2.6,"D",I116&lt;=2.5,"E")</f>
+        <f t="array" ref="J116">_xlfn.IFS(I116&gt;=3.7,"A",I116&gt;=3.3,"B",I116&gt;=2.8,"C",I116&gt;=2.5,"D",I116&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K116" s="9" t="str" cm="1">
@@ -5353,7 +5352,7 @@
         <v>3</v>
       </c>
       <c r="J117" s="9" t="str" cm="1">
-        <f t="array" ref="J117">_xlfn.IFS(I117&gt;=3.7,"A",I117&gt;=3.3,"B",I117&gt;=2.9,"C",I117&gt;=2.6,"D",I117&lt;=2.5,"E")</f>
+        <f t="array" ref="J117">_xlfn.IFS(I117&gt;=3.7,"A",I117&gt;=3.3,"B",I117&gt;=2.8,"C",I117&gt;=2.5,"D",I117&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K117" s="9" t="str" cm="1">
@@ -5394,7 +5393,7 @@
         <v>3</v>
       </c>
       <c r="J118" s="9" t="str" cm="1">
-        <f t="array" ref="J118">_xlfn.IFS(I118&gt;=3.7,"A",I118&gt;=3.3,"B",I118&gt;=2.9,"C",I118&gt;=2.6,"D",I118&lt;=2.5,"E")</f>
+        <f t="array" ref="J118">_xlfn.IFS(I118&gt;=3.7,"A",I118&gt;=3.3,"B",I118&gt;=2.8,"C",I118&gt;=2.5,"D",I118&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K118" s="9" t="str" cm="1">
@@ -5435,7 +5434,7 @@
         <v>3</v>
       </c>
       <c r="J119" s="9" t="str" cm="1">
-        <f t="array" ref="J119">_xlfn.IFS(I119&gt;=3.7,"A",I119&gt;=3.3,"B",I119&gt;=2.9,"C",I119&gt;=2.6,"D",I119&lt;=2.5,"E")</f>
+        <f t="array" ref="J119">_xlfn.IFS(I119&gt;=3.7,"A",I119&gt;=3.3,"B",I119&gt;=2.8,"C",I119&gt;=2.5,"D",I119&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K119" s="9" t="str" cm="1">
@@ -5476,7 +5475,7 @@
         <v>3</v>
       </c>
       <c r="J120" s="9" t="str" cm="1">
-        <f t="array" ref="J120">_xlfn.IFS(I120&gt;=3.7,"A",I120&gt;=3.3,"B",I120&gt;=2.9,"C",I120&gt;=2.6,"D",I120&lt;=2.5,"E")</f>
+        <f t="array" ref="J120">_xlfn.IFS(I120&gt;=3.7,"A",I120&gt;=3.3,"B",I120&gt;=2.8,"C",I120&gt;=2.5,"D",I120&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K120" s="9" t="str" cm="1">
@@ -5517,7 +5516,7 @@
         <v>3</v>
       </c>
       <c r="J121" s="9" t="str" cm="1">
-        <f t="array" ref="J121">_xlfn.IFS(I121&gt;=3.7,"A",I121&gt;=3.3,"B",I121&gt;=2.9,"C",I121&gt;=2.6,"D",I121&lt;=2.5,"E")</f>
+        <f t="array" ref="J121">_xlfn.IFS(I121&gt;=3.7,"A",I121&gt;=3.3,"B",I121&gt;=2.8,"C",I121&gt;=2.5,"D",I121&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K121" s="9" t="str" cm="1">
@@ -5558,7 +5557,7 @@
         <v>3</v>
       </c>
       <c r="J122" s="9" t="str" cm="1">
-        <f t="array" ref="J122">_xlfn.IFS(I122&gt;=3.7,"A",I122&gt;=3.3,"B",I122&gt;=2.9,"C",I122&gt;=2.6,"D",I122&lt;=2.5,"E")</f>
+        <f t="array" ref="J122">_xlfn.IFS(I122&gt;=3.7,"A",I122&gt;=3.3,"B",I122&gt;=2.8,"C",I122&gt;=2.5,"D",I122&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K122" s="9" t="str" cm="1">
@@ -5599,7 +5598,7 @@
         <v>3</v>
       </c>
       <c r="J123" s="9" t="str" cm="1">
-        <f t="array" ref="J123">_xlfn.IFS(I123&gt;=3.7,"A",I123&gt;=3.3,"B",I123&gt;=2.9,"C",I123&gt;=2.6,"D",I123&lt;=2.5,"E")</f>
+        <f t="array" ref="J123">_xlfn.IFS(I123&gt;=3.7,"A",I123&gt;=3.3,"B",I123&gt;=2.8,"C",I123&gt;=2.5,"D",I123&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K123" s="9" t="str" cm="1">
@@ -5640,7 +5639,7 @@
         <v>2.9</v>
       </c>
       <c r="J124" s="9" t="str" cm="1">
-        <f t="array" ref="J124">_xlfn.IFS(I124&gt;=3.7,"A",I124&gt;=3.3,"B",I124&gt;=2.9,"C",I124&gt;=2.6,"D",I124&lt;=2.5,"E")</f>
+        <f t="array" ref="J124">_xlfn.IFS(I124&gt;=3.7,"A",I124&gt;=3.3,"B",I124&gt;=2.8,"C",I124&gt;=2.5,"D",I124&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K124" s="9" t="str" cm="1">
@@ -5681,7 +5680,7 @@
         <v>2.9</v>
       </c>
       <c r="J125" s="9" t="str" cm="1">
-        <f t="array" ref="J125">_xlfn.IFS(I125&gt;=3.7,"A",I125&gt;=3.3,"B",I125&gt;=2.9,"C",I125&gt;=2.6,"D",I125&lt;=2.5,"E")</f>
+        <f t="array" ref="J125">_xlfn.IFS(I125&gt;=3.7,"A",I125&gt;=3.3,"B",I125&gt;=2.8,"C",I125&gt;=2.5,"D",I125&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K125" s="9" t="str" cm="1">
@@ -5722,7 +5721,7 @@
         <v>2.9</v>
       </c>
       <c r="J126" s="9" t="str" cm="1">
-        <f t="array" ref="J126">_xlfn.IFS(I126&gt;=3.7,"A",I126&gt;=3.3,"B",I126&gt;=2.9,"C",I126&gt;=2.6,"D",I126&lt;=2.5,"E")</f>
+        <f t="array" ref="J126">_xlfn.IFS(I126&gt;=3.7,"A",I126&gt;=3.3,"B",I126&gt;=2.8,"C",I126&gt;=2.5,"D",I126&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K126" s="9" t="str" cm="1">
@@ -5763,7 +5762,7 @@
         <v>2.9</v>
       </c>
       <c r="J127" s="9" t="str" cm="1">
-        <f t="array" ref="J127">_xlfn.IFS(I127&gt;=3.7,"A",I127&gt;=3.3,"B",I127&gt;=2.9,"C",I127&gt;=2.6,"D",I127&lt;=2.5,"E")</f>
+        <f t="array" ref="J127">_xlfn.IFS(I127&gt;=3.7,"A",I127&gt;=3.3,"B",I127&gt;=2.8,"C",I127&gt;=2.5,"D",I127&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K127" s="9" t="str" cm="1">
@@ -5804,7 +5803,7 @@
         <v>2.9</v>
       </c>
       <c r="J128" s="9" t="str" cm="1">
-        <f t="array" ref="J128">_xlfn.IFS(I128&gt;=3.7,"A",I128&gt;=3.3,"B",I128&gt;=2.9,"C",I128&gt;=2.6,"D",I128&lt;=2.5,"E")</f>
+        <f t="array" ref="J128">_xlfn.IFS(I128&gt;=3.7,"A",I128&gt;=3.3,"B",I128&gt;=2.8,"C",I128&gt;=2.5,"D",I128&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K128" s="9" t="str" cm="1">
@@ -5845,7 +5844,7 @@
         <v>2.9</v>
       </c>
       <c r="J129" s="9" t="str" cm="1">
-        <f t="array" ref="J129">_xlfn.IFS(I129&gt;=3.7,"A",I129&gt;=3.3,"B",I129&gt;=2.9,"C",I129&gt;=2.6,"D",I129&lt;=2.5,"E")</f>
+        <f t="array" ref="J129">_xlfn.IFS(I129&gt;=3.7,"A",I129&gt;=3.3,"B",I129&gt;=2.8,"C",I129&gt;=2.5,"D",I129&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K129" s="9" t="str" cm="1">
@@ -5886,7 +5885,7 @@
         <v>2.9</v>
       </c>
       <c r="J130" s="9" t="str" cm="1">
-        <f t="array" ref="J130">_xlfn.IFS(I130&gt;=3.7,"A",I130&gt;=3.3,"B",I130&gt;=2.9,"C",I130&gt;=2.6,"D",I130&lt;=2.5,"E")</f>
+        <f t="array" ref="J130">_xlfn.IFS(I130&gt;=3.7,"A",I130&gt;=3.3,"B",I130&gt;=2.8,"C",I130&gt;=2.5,"D",I130&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K130" s="9" t="str" cm="1">
@@ -5927,7 +5926,7 @@
         <v>2.9</v>
       </c>
       <c r="J131" s="9" t="str" cm="1">
-        <f t="array" ref="J131">_xlfn.IFS(I131&gt;=3.7,"A",I131&gt;=3.3,"B",I131&gt;=2.9,"C",I131&gt;=2.6,"D",I131&lt;=2.5,"E")</f>
+        <f t="array" ref="J131">_xlfn.IFS(I131&gt;=3.7,"A",I131&gt;=3.3,"B",I131&gt;=2.8,"C",I131&gt;=2.5,"D",I131&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K131" s="9" t="str" cm="1">
@@ -5968,7 +5967,7 @@
         <v>2.9</v>
       </c>
       <c r="J132" s="9" t="str" cm="1">
-        <f t="array" ref="J132">_xlfn.IFS(I132&gt;=3.7,"A",I132&gt;=3.3,"B",I132&gt;=2.9,"C",I132&gt;=2.6,"D",I132&lt;=2.5,"E")</f>
+        <f t="array" ref="J132">_xlfn.IFS(I132&gt;=3.7,"A",I132&gt;=3.3,"B",I132&gt;=2.8,"C",I132&gt;=2.5,"D",I132&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K132" s="9" t="str" cm="1">
@@ -6009,7 +6008,7 @@
         <v>2.9</v>
       </c>
       <c r="J133" s="9" t="str" cm="1">
-        <f t="array" ref="J133">_xlfn.IFS(I133&gt;=3.7,"A",I133&gt;=3.3,"B",I133&gt;=2.9,"C",I133&gt;=2.6,"D",I133&lt;=2.5,"E")</f>
+        <f t="array" ref="J133">_xlfn.IFS(I133&gt;=3.7,"A",I133&gt;=3.3,"B",I133&gt;=2.8,"C",I133&gt;=2.5,"D",I133&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K133" s="9" t="str" cm="1">
@@ -6050,7 +6049,7 @@
         <v>2.9</v>
       </c>
       <c r="J134" s="9" t="str" cm="1">
-        <f t="array" ref="J134">_xlfn.IFS(I134&gt;=3.7,"A",I134&gt;=3.3,"B",I134&gt;=2.9,"C",I134&gt;=2.6,"D",I134&lt;=2.5,"E")</f>
+        <f t="array" ref="J134">_xlfn.IFS(I134&gt;=3.7,"A",I134&gt;=3.3,"B",I134&gt;=2.8,"C",I134&gt;=2.5,"D",I134&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K134" s="9" t="str" cm="1">
@@ -6091,7 +6090,7 @@
         <v>2.9</v>
       </c>
       <c r="J135" s="9" t="str" cm="1">
-        <f t="array" ref="J135">_xlfn.IFS(I135&gt;=3.7,"A",I135&gt;=3.3,"B",I135&gt;=2.9,"C",I135&gt;=2.6,"D",I135&lt;=2.5,"E")</f>
+        <f t="array" ref="J135">_xlfn.IFS(I135&gt;=3.7,"A",I135&gt;=3.3,"B",I135&gt;=2.8,"C",I135&gt;=2.5,"D",I135&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K135" s="9" t="str" cm="1">
@@ -6132,7 +6131,7 @@
         <v>2.9</v>
       </c>
       <c r="J136" s="9" t="str" cm="1">
-        <f t="array" ref="J136">_xlfn.IFS(I136&gt;=3.7,"A",I136&gt;=3.3,"B",I136&gt;=2.9,"C",I136&gt;=2.6,"D",I136&lt;=2.5,"E")</f>
+        <f t="array" ref="J136">_xlfn.IFS(I136&gt;=3.7,"A",I136&gt;=3.3,"B",I136&gt;=2.8,"C",I136&gt;=2.5,"D",I136&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K136" s="9" t="str" cm="1">
@@ -6173,7 +6172,7 @@
         <v>2.9</v>
       </c>
       <c r="J137" s="9" t="str" cm="1">
-        <f t="array" ref="J137">_xlfn.IFS(I137&gt;=3.7,"A",I137&gt;=3.3,"B",I137&gt;=2.9,"C",I137&gt;=2.6,"D",I137&lt;=2.5,"E")</f>
+        <f t="array" ref="J137">_xlfn.IFS(I137&gt;=3.7,"A",I137&gt;=3.3,"B",I137&gt;=2.8,"C",I137&gt;=2.5,"D",I137&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K137" s="9" t="str" cm="1">
@@ -6214,7 +6213,7 @@
         <v>2.9</v>
       </c>
       <c r="J138" s="9" t="str" cm="1">
-        <f t="array" ref="J138">_xlfn.IFS(I138&gt;=3.7,"A",I138&gt;=3.3,"B",I138&gt;=2.9,"C",I138&gt;=2.6,"D",I138&lt;=2.5,"E")</f>
+        <f t="array" ref="J138">_xlfn.IFS(I138&gt;=3.7,"A",I138&gt;=3.3,"B",I138&gt;=2.8,"C",I138&gt;=2.5,"D",I138&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K138" s="9" t="str" cm="1">
@@ -6255,7 +6254,7 @@
         <v>2.9</v>
       </c>
       <c r="J139" s="9" t="str" cm="1">
-        <f t="array" ref="J139">_xlfn.IFS(I139&gt;=3.7,"A",I139&gt;=3.3,"B",I139&gt;=2.9,"C",I139&gt;=2.6,"D",I139&lt;=2.5,"E")</f>
+        <f t="array" ref="J139">_xlfn.IFS(I139&gt;=3.7,"A",I139&gt;=3.3,"B",I139&gt;=2.8,"C",I139&gt;=2.5,"D",I139&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K139" s="9" t="str" cm="1">
@@ -6296,7 +6295,7 @@
         <v>2.9</v>
       </c>
       <c r="J140" s="9" t="str" cm="1">
-        <f t="array" ref="J140">_xlfn.IFS(I140&gt;=3.7,"A",I140&gt;=3.3,"B",I140&gt;=2.9,"C",I140&gt;=2.6,"D",I140&lt;=2.5,"E")</f>
+        <f t="array" ref="J140">_xlfn.IFS(I140&gt;=3.7,"A",I140&gt;=3.3,"B",I140&gt;=2.8,"C",I140&gt;=2.5,"D",I140&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K140" s="9" t="str" cm="1">
@@ -6337,7 +6336,7 @@
         <v>2.9</v>
       </c>
       <c r="J141" s="9" t="str" cm="1">
-        <f t="array" ref="J141">_xlfn.IFS(I141&gt;=3.7,"A",I141&gt;=3.3,"B",I141&gt;=2.9,"C",I141&gt;=2.6,"D",I141&lt;=2.5,"E")</f>
+        <f t="array" ref="J141">_xlfn.IFS(I141&gt;=3.7,"A",I141&gt;=3.3,"B",I141&gt;=2.8,"C",I141&gt;=2.5,"D",I141&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K141" s="9" t="str" cm="1">
@@ -6378,7 +6377,7 @@
         <v>2.9</v>
       </c>
       <c r="J142" s="9" t="str" cm="1">
-        <f t="array" ref="J142">_xlfn.IFS(I142&gt;=3.7,"A",I142&gt;=3.3,"B",I142&gt;=2.9,"C",I142&gt;=2.6,"D",I142&lt;=2.5,"E")</f>
+        <f t="array" ref="J142">_xlfn.IFS(I142&gt;=3.7,"A",I142&gt;=3.3,"B",I142&gt;=2.8,"C",I142&gt;=2.5,"D",I142&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K142" s="9" t="str" cm="1">
@@ -6419,7 +6418,7 @@
         <v>2.9</v>
       </c>
       <c r="J143" s="9" t="str" cm="1">
-        <f t="array" ref="J143">_xlfn.IFS(I143&gt;=3.7,"A",I143&gt;=3.3,"B",I143&gt;=2.9,"C",I143&gt;=2.6,"D",I143&lt;=2.5,"E")</f>
+        <f t="array" ref="J143">_xlfn.IFS(I143&gt;=3.7,"A",I143&gt;=3.3,"B",I143&gt;=2.8,"C",I143&gt;=2.5,"D",I143&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K143" s="9" t="str" cm="1">
@@ -6460,7 +6459,7 @@
         <v>2.9</v>
       </c>
       <c r="J144" s="9" t="str" cm="1">
-        <f t="array" ref="J144">_xlfn.IFS(I144&gt;=3.7,"A",I144&gt;=3.3,"B",I144&gt;=2.9,"C",I144&gt;=2.6,"D",I144&lt;=2.5,"E")</f>
+        <f t="array" ref="J144">_xlfn.IFS(I144&gt;=3.7,"A",I144&gt;=3.3,"B",I144&gt;=2.8,"C",I144&gt;=2.5,"D",I144&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K144" s="9" t="str" cm="1">
@@ -6501,7 +6500,7 @@
         <v>2.9</v>
       </c>
       <c r="J145" s="9" t="str" cm="1">
-        <f t="array" ref="J145">_xlfn.IFS(I145&gt;=3.7,"A",I145&gt;=3.3,"B",I145&gt;=2.9,"C",I145&gt;=2.6,"D",I145&lt;=2.5,"E")</f>
+        <f t="array" ref="J145">_xlfn.IFS(I145&gt;=3.7,"A",I145&gt;=3.3,"B",I145&gt;=2.8,"C",I145&gt;=2.5,"D",I145&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K145" s="9" t="str" cm="1">
@@ -6542,7 +6541,7 @@
         <v>2.9</v>
       </c>
       <c r="J146" s="9" t="str" cm="1">
-        <f t="array" ref="J146">_xlfn.IFS(I146&gt;=3.7,"A",I146&gt;=3.3,"B",I146&gt;=2.9,"C",I146&gt;=2.6,"D",I146&lt;=2.5,"E")</f>
+        <f t="array" ref="J146">_xlfn.IFS(I146&gt;=3.7,"A",I146&gt;=3.3,"B",I146&gt;=2.8,"C",I146&gt;=2.5,"D",I146&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K146" s="9" t="str" cm="1">
@@ -6583,7 +6582,7 @@
         <v>2.9</v>
       </c>
       <c r="J147" s="9" t="str" cm="1">
-        <f t="array" ref="J147">_xlfn.IFS(I147&gt;=3.7,"A",I147&gt;=3.3,"B",I147&gt;=2.9,"C",I147&gt;=2.6,"D",I147&lt;=2.5,"E")</f>
+        <f t="array" ref="J147">_xlfn.IFS(I147&gt;=3.7,"A",I147&gt;=3.3,"B",I147&gt;=2.8,"C",I147&gt;=2.5,"D",I147&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K147" s="9" t="str" cm="1">
@@ -6624,7 +6623,7 @@
         <v>2.9</v>
       </c>
       <c r="J148" s="9" t="str" cm="1">
-        <f t="array" ref="J148">_xlfn.IFS(I148&gt;=3.7,"A",I148&gt;=3.3,"B",I148&gt;=2.9,"C",I148&gt;=2.6,"D",I148&lt;=2.5,"E")</f>
+        <f t="array" ref="J148">_xlfn.IFS(I148&gt;=3.7,"A",I148&gt;=3.3,"B",I148&gt;=2.8,"C",I148&gt;=2.5,"D",I148&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K148" s="9" t="str" cm="1">
@@ -6665,7 +6664,7 @@
         <v>2.9</v>
       </c>
       <c r="J149" s="9" t="str" cm="1">
-        <f t="array" ref="J149">_xlfn.IFS(I149&gt;=3.7,"A",I149&gt;=3.3,"B",I149&gt;=2.9,"C",I149&gt;=2.6,"D",I149&lt;=2.5,"E")</f>
+        <f t="array" ref="J149">_xlfn.IFS(I149&gt;=3.7,"A",I149&gt;=3.3,"B",I149&gt;=2.8,"C",I149&gt;=2.5,"D",I149&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K149" s="9" t="str" cm="1">
@@ -6706,7 +6705,7 @@
         <v>2.9</v>
       </c>
       <c r="J150" s="9" t="str" cm="1">
-        <f t="array" ref="J150">_xlfn.IFS(I150&gt;=3.7,"A",I150&gt;=3.3,"B",I150&gt;=2.9,"C",I150&gt;=2.6,"D",I150&lt;=2.5,"E")</f>
+        <f t="array" ref="J150">_xlfn.IFS(I150&gt;=3.7,"A",I150&gt;=3.3,"B",I150&gt;=2.8,"C",I150&gt;=2.5,"D",I150&lt;=2.4,"E")</f>
         <v>C</v>
       </c>
       <c r="K150" s="9" t="str" cm="1">
@@ -6747,12 +6746,12 @@
         <v>2.8</v>
       </c>
       <c r="J151" s="9" t="str" cm="1">
-        <f t="array" ref="J151">_xlfn.IFS(I151&gt;=3.7,"A",I151&gt;=3.3,"B",I151&gt;=2.9,"C",I151&gt;=2.6,"D",I151&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J151">_xlfn.IFS(I151&gt;=3.7,"A",I151&gt;=3.3,"B",I151&gt;=2.8,"C",I151&gt;=2.5,"D",I151&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K151" s="9" t="str" cm="1">
         <f t="array" ref="K151">_xlfn.IFS(J151="A","LULUS",J151="B","LULUS",J151="C","LULUS",J151="D","TIDAK LULUS",J151="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L151" s="2"/>
       <c r="Q151"/>
@@ -6788,12 +6787,12 @@
         <v>2.8</v>
       </c>
       <c r="J152" s="9" t="str" cm="1">
-        <f t="array" ref="J152">_xlfn.IFS(I152&gt;=3.7,"A",I152&gt;=3.3,"B",I152&gt;=2.9,"C",I152&gt;=2.6,"D",I152&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J152">_xlfn.IFS(I152&gt;=3.7,"A",I152&gt;=3.3,"B",I152&gt;=2.8,"C",I152&gt;=2.5,"D",I152&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K152" s="9" t="str" cm="1">
         <f t="array" ref="K152">_xlfn.IFS(J152="A","LULUS",J152="B","LULUS",J152="C","LULUS",J152="D","TIDAK LULUS",J152="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L152" s="2"/>
       <c r="Q152"/>
@@ -6829,12 +6828,12 @@
         <v>2.8</v>
       </c>
       <c r="J153" s="9" t="str" cm="1">
-        <f t="array" ref="J153">_xlfn.IFS(I153&gt;=3.7,"A",I153&gt;=3.3,"B",I153&gt;=2.9,"C",I153&gt;=2.6,"D",I153&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J153">_xlfn.IFS(I153&gt;=3.7,"A",I153&gt;=3.3,"B",I153&gt;=2.8,"C",I153&gt;=2.5,"D",I153&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K153" s="9" t="str" cm="1">
         <f t="array" ref="K153">_xlfn.IFS(J153="A","LULUS",J153="B","LULUS",J153="C","LULUS",J153="D","TIDAK LULUS",J153="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L153" s="2"/>
       <c r="Q153"/>
@@ -6870,12 +6869,12 @@
         <v>2.8</v>
       </c>
       <c r="J154" s="9" t="str" cm="1">
-        <f t="array" ref="J154">_xlfn.IFS(I154&gt;=3.7,"A",I154&gt;=3.3,"B",I154&gt;=2.9,"C",I154&gt;=2.6,"D",I154&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J154">_xlfn.IFS(I154&gt;=3.7,"A",I154&gt;=3.3,"B",I154&gt;=2.8,"C",I154&gt;=2.5,"D",I154&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K154" s="9" t="str" cm="1">
         <f t="array" ref="K154">_xlfn.IFS(J154="A","LULUS",J154="B","LULUS",J154="C","LULUS",J154="D","TIDAK LULUS",J154="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L154" s="2"/>
       <c r="Q154"/>
@@ -6911,12 +6910,12 @@
         <v>2.8</v>
       </c>
       <c r="J155" s="9" t="str" cm="1">
-        <f t="array" ref="J155">_xlfn.IFS(I155&gt;=3.7,"A",I155&gt;=3.3,"B",I155&gt;=2.9,"C",I155&gt;=2.6,"D",I155&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J155">_xlfn.IFS(I155&gt;=3.7,"A",I155&gt;=3.3,"B",I155&gt;=2.8,"C",I155&gt;=2.5,"D",I155&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K155" s="9" t="str" cm="1">
         <f t="array" ref="K155">_xlfn.IFS(J155="A","LULUS",J155="B","LULUS",J155="C","LULUS",J155="D","TIDAK LULUS",J155="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L155" s="2"/>
       <c r="Q155"/>
@@ -6952,12 +6951,12 @@
         <v>2.8</v>
       </c>
       <c r="J156" s="9" t="str" cm="1">
-        <f t="array" ref="J156">_xlfn.IFS(I156&gt;=3.7,"A",I156&gt;=3.3,"B",I156&gt;=2.9,"C",I156&gt;=2.6,"D",I156&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J156">_xlfn.IFS(I156&gt;=3.7,"A",I156&gt;=3.3,"B",I156&gt;=2.8,"C",I156&gt;=2.5,"D",I156&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K156" s="9" t="str" cm="1">
         <f t="array" ref="K156">_xlfn.IFS(J156="A","LULUS",J156="B","LULUS",J156="C","LULUS",J156="D","TIDAK LULUS",J156="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L156" s="2"/>
       <c r="Q156"/>
@@ -6993,12 +6992,12 @@
         <v>2.8</v>
       </c>
       <c r="J157" s="9" t="str" cm="1">
-        <f t="array" ref="J157">_xlfn.IFS(I157&gt;=3.7,"A",I157&gt;=3.3,"B",I157&gt;=2.9,"C",I157&gt;=2.6,"D",I157&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J157">_xlfn.IFS(I157&gt;=3.7,"A",I157&gt;=3.3,"B",I157&gt;=2.8,"C",I157&gt;=2.5,"D",I157&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K157" s="9" t="str" cm="1">
         <f t="array" ref="K157">_xlfn.IFS(J157="A","LULUS",J157="B","LULUS",J157="C","LULUS",J157="D","TIDAK LULUS",J157="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L157" s="2"/>
       <c r="Q157"/>
@@ -7034,12 +7033,12 @@
         <v>2.8</v>
       </c>
       <c r="J158" s="9" t="str" cm="1">
-        <f t="array" ref="J158">_xlfn.IFS(I158&gt;=3.7,"A",I158&gt;=3.3,"B",I158&gt;=2.9,"C",I158&gt;=2.6,"D",I158&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J158">_xlfn.IFS(I158&gt;=3.7,"A",I158&gt;=3.3,"B",I158&gt;=2.8,"C",I158&gt;=2.5,"D",I158&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K158" s="9" t="str" cm="1">
         <f t="array" ref="K158">_xlfn.IFS(J158="A","LULUS",J158="B","LULUS",J158="C","LULUS",J158="D","TIDAK LULUS",J158="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L158" s="2"/>
       <c r="Q158"/>
@@ -7075,12 +7074,12 @@
         <v>2.8</v>
       </c>
       <c r="J159" s="9" t="str" cm="1">
-        <f t="array" ref="J159">_xlfn.IFS(I159&gt;=3.7,"A",I159&gt;=3.3,"B",I159&gt;=2.9,"C",I159&gt;=2.6,"D",I159&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J159">_xlfn.IFS(I159&gt;=3.7,"A",I159&gt;=3.3,"B",I159&gt;=2.8,"C",I159&gt;=2.5,"D",I159&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K159" s="9" t="str" cm="1">
         <f t="array" ref="K159">_xlfn.IFS(J159="A","LULUS",J159="B","LULUS",J159="C","LULUS",J159="D","TIDAK LULUS",J159="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L159" s="2"/>
       <c r="Q159"/>
@@ -7116,12 +7115,12 @@
         <v>2.8</v>
       </c>
       <c r="J160" s="9" t="str" cm="1">
-        <f t="array" ref="J160">_xlfn.IFS(I160&gt;=3.7,"A",I160&gt;=3.3,"B",I160&gt;=2.9,"C",I160&gt;=2.6,"D",I160&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J160">_xlfn.IFS(I160&gt;=3.7,"A",I160&gt;=3.3,"B",I160&gt;=2.8,"C",I160&gt;=2.5,"D",I160&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K160" s="9" t="str" cm="1">
         <f t="array" ref="K160">_xlfn.IFS(J160="A","LULUS",J160="B","LULUS",J160="C","LULUS",J160="D","TIDAK LULUS",J160="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L160" s="2"/>
       <c r="Q160"/>
@@ -7157,12 +7156,12 @@
         <v>2.8</v>
       </c>
       <c r="J161" s="9" t="str" cm="1">
-        <f t="array" ref="J161">_xlfn.IFS(I161&gt;=3.7,"A",I161&gt;=3.3,"B",I161&gt;=2.9,"C",I161&gt;=2.6,"D",I161&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J161">_xlfn.IFS(I161&gt;=3.7,"A",I161&gt;=3.3,"B",I161&gt;=2.8,"C",I161&gt;=2.5,"D",I161&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K161" s="9" t="str" cm="1">
         <f t="array" ref="K161">_xlfn.IFS(J161="A","LULUS",J161="B","LULUS",J161="C","LULUS",J161="D","TIDAK LULUS",J161="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L161" s="2"/>
       <c r="Q161"/>
@@ -7198,12 +7197,12 @@
         <v>2.8</v>
       </c>
       <c r="J162" s="9" t="str" cm="1">
-        <f t="array" ref="J162">_xlfn.IFS(I162&gt;=3.7,"A",I162&gt;=3.3,"B",I162&gt;=2.9,"C",I162&gt;=2.6,"D",I162&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J162">_xlfn.IFS(I162&gt;=3.7,"A",I162&gt;=3.3,"B",I162&gt;=2.8,"C",I162&gt;=2.5,"D",I162&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K162" s="9" t="str" cm="1">
         <f t="array" ref="K162">_xlfn.IFS(J162="A","LULUS",J162="B","LULUS",J162="C","LULUS",J162="D","TIDAK LULUS",J162="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L162" s="2"/>
       <c r="Q162"/>
@@ -7239,12 +7238,12 @@
         <v>2.8</v>
       </c>
       <c r="J163" s="9" t="str" cm="1">
-        <f t="array" ref="J163">_xlfn.IFS(I163&gt;=3.7,"A",I163&gt;=3.3,"B",I163&gt;=2.9,"C",I163&gt;=2.6,"D",I163&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J163">_xlfn.IFS(I163&gt;=3.7,"A",I163&gt;=3.3,"B",I163&gt;=2.8,"C",I163&gt;=2.5,"D",I163&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K163" s="9" t="str" cm="1">
         <f t="array" ref="K163">_xlfn.IFS(J163="A","LULUS",J163="B","LULUS",J163="C","LULUS",J163="D","TIDAK LULUS",J163="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L163" s="2"/>
       <c r="Q163"/>
@@ -7280,12 +7279,12 @@
         <v>2.8</v>
       </c>
       <c r="J164" s="9" t="str" cm="1">
-        <f t="array" ref="J164">_xlfn.IFS(I164&gt;=3.7,"A",I164&gt;=3.3,"B",I164&gt;=2.9,"C",I164&gt;=2.6,"D",I164&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J164">_xlfn.IFS(I164&gt;=3.7,"A",I164&gt;=3.3,"B",I164&gt;=2.8,"C",I164&gt;=2.5,"D",I164&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K164" s="9" t="str" cm="1">
         <f t="array" ref="K164">_xlfn.IFS(J164="A","LULUS",J164="B","LULUS",J164="C","LULUS",J164="D","TIDAK LULUS",J164="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L164" s="2"/>
       <c r="Q164"/>
@@ -7321,12 +7320,12 @@
         <v>2.8</v>
       </c>
       <c r="J165" s="9" t="str" cm="1">
-        <f t="array" ref="J165">_xlfn.IFS(I165&gt;=3.7,"A",I165&gt;=3.3,"B",I165&gt;=2.9,"C",I165&gt;=2.6,"D",I165&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J165">_xlfn.IFS(I165&gt;=3.7,"A",I165&gt;=3.3,"B",I165&gt;=2.8,"C",I165&gt;=2.5,"D",I165&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K165" s="9" t="str" cm="1">
         <f t="array" ref="K165">_xlfn.IFS(J165="A","LULUS",J165="B","LULUS",J165="C","LULUS",J165="D","TIDAK LULUS",J165="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L165" s="2"/>
       <c r="Q165"/>
@@ -7362,12 +7361,12 @@
         <v>2.8</v>
       </c>
       <c r="J166" s="9" t="str" cm="1">
-        <f t="array" ref="J166">_xlfn.IFS(I166&gt;=3.7,"A",I166&gt;=3.3,"B",I166&gt;=2.9,"C",I166&gt;=2.6,"D",I166&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J166">_xlfn.IFS(I166&gt;=3.7,"A",I166&gt;=3.3,"B",I166&gt;=2.8,"C",I166&gt;=2.5,"D",I166&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K166" s="9" t="str" cm="1">
         <f t="array" ref="K166">_xlfn.IFS(J166="A","LULUS",J166="B","LULUS",J166="C","LULUS",J166="D","TIDAK LULUS",J166="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L166" s="2"/>
       <c r="Q166"/>
@@ -7403,12 +7402,12 @@
         <v>2.8</v>
       </c>
       <c r="J167" s="9" t="str" cm="1">
-        <f t="array" ref="J167">_xlfn.IFS(I167&gt;=3.7,"A",I167&gt;=3.3,"B",I167&gt;=2.9,"C",I167&gt;=2.6,"D",I167&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J167">_xlfn.IFS(I167&gt;=3.7,"A",I167&gt;=3.3,"B",I167&gt;=2.8,"C",I167&gt;=2.5,"D",I167&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K167" s="9" t="str" cm="1">
         <f t="array" ref="K167">_xlfn.IFS(J167="A","LULUS",J167="B","LULUS",J167="C","LULUS",J167="D","TIDAK LULUS",J167="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L167" s="2"/>
       <c r="Q167"/>
@@ -7444,12 +7443,12 @@
         <v>2.8</v>
       </c>
       <c r="J168" s="9" t="str" cm="1">
-        <f t="array" ref="J168">_xlfn.IFS(I168&gt;=3.7,"A",I168&gt;=3.3,"B",I168&gt;=2.9,"C",I168&gt;=2.6,"D",I168&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J168">_xlfn.IFS(I168&gt;=3.7,"A",I168&gt;=3.3,"B",I168&gt;=2.8,"C",I168&gt;=2.5,"D",I168&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K168" s="9" t="str" cm="1">
         <f t="array" ref="K168">_xlfn.IFS(J168="A","LULUS",J168="B","LULUS",J168="C","LULUS",J168="D","TIDAK LULUS",J168="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L168" s="2"/>
       <c r="Q168"/>
@@ -7485,12 +7484,12 @@
         <v>2.8</v>
       </c>
       <c r="J169" s="9" t="str" cm="1">
-        <f t="array" ref="J169">_xlfn.IFS(I169&gt;=3.7,"A",I169&gt;=3.3,"B",I169&gt;=2.9,"C",I169&gt;=2.6,"D",I169&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J169">_xlfn.IFS(I169&gt;=3.7,"A",I169&gt;=3.3,"B",I169&gt;=2.8,"C",I169&gt;=2.5,"D",I169&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K169" s="9" t="str" cm="1">
         <f t="array" ref="K169">_xlfn.IFS(J169="A","LULUS",J169="B","LULUS",J169="C","LULUS",J169="D","TIDAK LULUS",J169="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L169" s="2"/>
       <c r="Q169"/>
@@ -7526,12 +7525,12 @@
         <v>2.8</v>
       </c>
       <c r="J170" s="9" t="str" cm="1">
-        <f t="array" ref="J170">_xlfn.IFS(I170&gt;=3.7,"A",I170&gt;=3.3,"B",I170&gt;=2.9,"C",I170&gt;=2.6,"D",I170&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J170">_xlfn.IFS(I170&gt;=3.7,"A",I170&gt;=3.3,"B",I170&gt;=2.8,"C",I170&gt;=2.5,"D",I170&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K170" s="9" t="str" cm="1">
         <f t="array" ref="K170">_xlfn.IFS(J170="A","LULUS",J170="B","LULUS",J170="C","LULUS",J170="D","TIDAK LULUS",J170="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L170" s="2"/>
       <c r="Q170"/>
@@ -7567,12 +7566,12 @@
         <v>2.8</v>
       </c>
       <c r="J171" s="9" t="str" cm="1">
-        <f t="array" ref="J171">_xlfn.IFS(I171&gt;=3.7,"A",I171&gt;=3.3,"B",I171&gt;=2.9,"C",I171&gt;=2.6,"D",I171&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J171">_xlfn.IFS(I171&gt;=3.7,"A",I171&gt;=3.3,"B",I171&gt;=2.8,"C",I171&gt;=2.5,"D",I171&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K171" s="9" t="str" cm="1">
         <f t="array" ref="K171">_xlfn.IFS(J171="A","LULUS",J171="B","LULUS",J171="C","LULUS",J171="D","TIDAK LULUS",J171="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L171" s="2"/>
       <c r="Q171"/>
@@ -7608,12 +7607,12 @@
         <v>2.8</v>
       </c>
       <c r="J172" s="9" t="str" cm="1">
-        <f t="array" ref="J172">_xlfn.IFS(I172&gt;=3.7,"A",I172&gt;=3.3,"B",I172&gt;=2.9,"C",I172&gt;=2.6,"D",I172&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J172">_xlfn.IFS(I172&gt;=3.7,"A",I172&gt;=3.3,"B",I172&gt;=2.8,"C",I172&gt;=2.5,"D",I172&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K172" s="9" t="str" cm="1">
         <f t="array" ref="K172">_xlfn.IFS(J172="A","LULUS",J172="B","LULUS",J172="C","LULUS",J172="D","TIDAK LULUS",J172="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L172" s="2"/>
       <c r="Q172"/>
@@ -7649,12 +7648,12 @@
         <v>2.8</v>
       </c>
       <c r="J173" s="9" t="str" cm="1">
-        <f t="array" ref="J173">_xlfn.IFS(I173&gt;=3.7,"A",I173&gt;=3.3,"B",I173&gt;=2.9,"C",I173&gt;=2.6,"D",I173&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J173">_xlfn.IFS(I173&gt;=3.7,"A",I173&gt;=3.3,"B",I173&gt;=2.8,"C",I173&gt;=2.5,"D",I173&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K173" s="9" t="str" cm="1">
         <f t="array" ref="K173">_xlfn.IFS(J173="A","LULUS",J173="B","LULUS",J173="C","LULUS",J173="D","TIDAK LULUS",J173="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L173" s="2"/>
       <c r="Q173"/>
@@ -7690,12 +7689,12 @@
         <v>2.8</v>
       </c>
       <c r="J174" s="9" t="str" cm="1">
-        <f t="array" ref="J174">_xlfn.IFS(I174&gt;=3.7,"A",I174&gt;=3.3,"B",I174&gt;=2.9,"C",I174&gt;=2.6,"D",I174&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J174">_xlfn.IFS(I174&gt;=3.7,"A",I174&gt;=3.3,"B",I174&gt;=2.8,"C",I174&gt;=2.5,"D",I174&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K174" s="9" t="str" cm="1">
         <f t="array" ref="K174">_xlfn.IFS(J174="A","LULUS",J174="B","LULUS",J174="C","LULUS",J174="D","TIDAK LULUS",J174="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L174" s="2"/>
       <c r="Q174"/>
@@ -7731,12 +7730,12 @@
         <v>2.8</v>
       </c>
       <c r="J175" s="9" t="str" cm="1">
-        <f t="array" ref="J175">_xlfn.IFS(I175&gt;=3.7,"A",I175&gt;=3.3,"B",I175&gt;=2.9,"C",I175&gt;=2.6,"D",I175&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J175">_xlfn.IFS(I175&gt;=3.7,"A",I175&gt;=3.3,"B",I175&gt;=2.8,"C",I175&gt;=2.5,"D",I175&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K175" s="9" t="str" cm="1">
         <f t="array" ref="K175">_xlfn.IFS(J175="A","LULUS",J175="B","LULUS",J175="C","LULUS",J175="D","TIDAK LULUS",J175="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L175" s="2"/>
       <c r="Q175"/>
@@ -7772,12 +7771,12 @@
         <v>2.8</v>
       </c>
       <c r="J176" s="9" t="str" cm="1">
-        <f t="array" ref="J176">_xlfn.IFS(I176&gt;=3.7,"A",I176&gt;=3.3,"B",I176&gt;=2.9,"C",I176&gt;=2.6,"D",I176&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J176">_xlfn.IFS(I176&gt;=3.7,"A",I176&gt;=3.3,"B",I176&gt;=2.8,"C",I176&gt;=2.5,"D",I176&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K176" s="9" t="str" cm="1">
         <f t="array" ref="K176">_xlfn.IFS(J176="A","LULUS",J176="B","LULUS",J176="C","LULUS",J176="D","TIDAK LULUS",J176="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L176" s="2"/>
       <c r="Q176"/>
@@ -7813,12 +7812,12 @@
         <v>2.8</v>
       </c>
       <c r="J177" s="9" t="str" cm="1">
-        <f t="array" ref="J177">_xlfn.IFS(I177&gt;=3.7,"A",I177&gt;=3.3,"B",I177&gt;=2.9,"C",I177&gt;=2.6,"D",I177&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J177">_xlfn.IFS(I177&gt;=3.7,"A",I177&gt;=3.3,"B",I177&gt;=2.8,"C",I177&gt;=2.5,"D",I177&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K177" s="9" t="str" cm="1">
         <f t="array" ref="K177">_xlfn.IFS(J177="A","LULUS",J177="B","LULUS",J177="C","LULUS",J177="D","TIDAK LULUS",J177="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L177" s="2"/>
       <c r="Q177"/>
@@ -7854,12 +7853,12 @@
         <v>2.8</v>
       </c>
       <c r="J178" s="9" t="str" cm="1">
-        <f t="array" ref="J178">_xlfn.IFS(I178&gt;=3.7,"A",I178&gt;=3.3,"B",I178&gt;=2.9,"C",I178&gt;=2.6,"D",I178&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J178">_xlfn.IFS(I178&gt;=3.7,"A",I178&gt;=3.3,"B",I178&gt;=2.8,"C",I178&gt;=2.5,"D",I178&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K178" s="9" t="str" cm="1">
         <f t="array" ref="K178">_xlfn.IFS(J178="A","LULUS",J178="B","LULUS",J178="C","LULUS",J178="D","TIDAK LULUS",J178="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L178" s="2"/>
       <c r="Q178"/>
@@ -7895,12 +7894,12 @@
         <v>2.8</v>
       </c>
       <c r="J179" s="9" t="str" cm="1">
-        <f t="array" ref="J179">_xlfn.IFS(I179&gt;=3.7,"A",I179&gt;=3.3,"B",I179&gt;=2.9,"C",I179&gt;=2.6,"D",I179&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J179">_xlfn.IFS(I179&gt;=3.7,"A",I179&gt;=3.3,"B",I179&gt;=2.8,"C",I179&gt;=2.5,"D",I179&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K179" s="9" t="str" cm="1">
         <f t="array" ref="K179">_xlfn.IFS(J179="A","LULUS",J179="B","LULUS",J179="C","LULUS",J179="D","TIDAK LULUS",J179="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L179" s="2"/>
       <c r="Q179"/>
@@ -7936,12 +7935,12 @@
         <v>2.8</v>
       </c>
       <c r="J180" s="9" t="str" cm="1">
-        <f t="array" ref="J180">_xlfn.IFS(I180&gt;=3.7,"A",I180&gt;=3.3,"B",I180&gt;=2.9,"C",I180&gt;=2.6,"D",I180&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J180">_xlfn.IFS(I180&gt;=3.7,"A",I180&gt;=3.3,"B",I180&gt;=2.8,"C",I180&gt;=2.5,"D",I180&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K180" s="9" t="str" cm="1">
         <f t="array" ref="K180">_xlfn.IFS(J180="A","LULUS",J180="B","LULUS",J180="C","LULUS",J180="D","TIDAK LULUS",J180="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L180" s="2"/>
       <c r="Q180"/>
@@ -7977,12 +7976,12 @@
         <v>2.8</v>
       </c>
       <c r="J181" s="9" t="str" cm="1">
-        <f t="array" ref="J181">_xlfn.IFS(I181&gt;=3.7,"A",I181&gt;=3.3,"B",I181&gt;=2.9,"C",I181&gt;=2.6,"D",I181&lt;=2.5,"E")</f>
-        <v>D</v>
+        <f t="array" ref="J181">_xlfn.IFS(I181&gt;=3.7,"A",I181&gt;=3.3,"B",I181&gt;=2.8,"C",I181&gt;=2.5,"D",I181&lt;=2.4,"E")</f>
+        <v>C</v>
       </c>
       <c r="K181" s="9" t="str" cm="1">
         <f t="array" ref="K181">_xlfn.IFS(J181="A","LULUS",J181="B","LULUS",J181="C","LULUS",J181="D","TIDAK LULUS",J181="E","TIDAK LULUS")</f>
-        <v>TIDAK LULUS</v>
+        <v>LULUS</v>
       </c>
       <c r="L181" s="2"/>
       <c r="Q181"/>
@@ -8018,7 +8017,7 @@
         <v>2.7</v>
       </c>
       <c r="J182" s="9" t="str" cm="1">
-        <f t="array" ref="J182">_xlfn.IFS(I182&gt;=3.7,"A",I182&gt;=3.3,"B",I182&gt;=2.9,"C",I182&gt;=2.6,"D",I182&lt;=2.5,"E")</f>
+        <f t="array" ref="J182">_xlfn.IFS(I182&gt;=3.7,"A",I182&gt;=3.3,"B",I182&gt;=2.8,"C",I182&gt;=2.5,"D",I182&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K182" s="9" t="str" cm="1">
@@ -8059,7 +8058,7 @@
         <v>2.7</v>
       </c>
       <c r="J183" s="9" t="str" cm="1">
-        <f t="array" ref="J183">_xlfn.IFS(I183&gt;=3.7,"A",I183&gt;=3.3,"B",I183&gt;=2.9,"C",I183&gt;=2.6,"D",I183&lt;=2.5,"E")</f>
+        <f t="array" ref="J183">_xlfn.IFS(I183&gt;=3.7,"A",I183&gt;=3.3,"B",I183&gt;=2.8,"C",I183&gt;=2.5,"D",I183&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K183" s="9" t="str" cm="1">
@@ -8100,7 +8099,7 @@
         <v>2.7</v>
       </c>
       <c r="J184" s="9" t="str" cm="1">
-        <f t="array" ref="J184">_xlfn.IFS(I184&gt;=3.7,"A",I184&gt;=3.3,"B",I184&gt;=2.9,"C",I184&gt;=2.6,"D",I184&lt;=2.5,"E")</f>
+        <f t="array" ref="J184">_xlfn.IFS(I184&gt;=3.7,"A",I184&gt;=3.3,"B",I184&gt;=2.8,"C",I184&gt;=2.5,"D",I184&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K184" s="9" t="str" cm="1">
@@ -8141,7 +8140,7 @@
         <v>2.7</v>
       </c>
       <c r="J185" s="9" t="str" cm="1">
-        <f t="array" ref="J185">_xlfn.IFS(I185&gt;=3.7,"A",I185&gt;=3.3,"B",I185&gt;=2.9,"C",I185&gt;=2.6,"D",I185&lt;=2.5,"E")</f>
+        <f t="array" ref="J185">_xlfn.IFS(I185&gt;=3.7,"A",I185&gt;=3.3,"B",I185&gt;=2.8,"C",I185&gt;=2.5,"D",I185&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K185" s="9" t="str" cm="1">
@@ -8182,7 +8181,7 @@
         <v>2.7</v>
       </c>
       <c r="J186" s="9" t="str" cm="1">
-        <f t="array" ref="J186">_xlfn.IFS(I186&gt;=3.7,"A",I186&gt;=3.3,"B",I186&gt;=2.9,"C",I186&gt;=2.6,"D",I186&lt;=2.5,"E")</f>
+        <f t="array" ref="J186">_xlfn.IFS(I186&gt;=3.7,"A",I186&gt;=3.3,"B",I186&gt;=2.8,"C",I186&gt;=2.5,"D",I186&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K186" s="9" t="str" cm="1">
@@ -8223,7 +8222,7 @@
         <v>2.7</v>
       </c>
       <c r="J187" s="9" t="str" cm="1">
-        <f t="array" ref="J187">_xlfn.IFS(I187&gt;=3.7,"A",I187&gt;=3.3,"B",I187&gt;=2.9,"C",I187&gt;=2.6,"D",I187&lt;=2.5,"E")</f>
+        <f t="array" ref="J187">_xlfn.IFS(I187&gt;=3.7,"A",I187&gt;=3.3,"B",I187&gt;=2.8,"C",I187&gt;=2.5,"D",I187&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K187" s="9" t="str" cm="1">
@@ -8264,7 +8263,7 @@
         <v>2.7</v>
       </c>
       <c r="J188" s="9" t="str" cm="1">
-        <f t="array" ref="J188">_xlfn.IFS(I188&gt;=3.7,"A",I188&gt;=3.3,"B",I188&gt;=2.9,"C",I188&gt;=2.6,"D",I188&lt;=2.5,"E")</f>
+        <f t="array" ref="J188">_xlfn.IFS(I188&gt;=3.7,"A",I188&gt;=3.3,"B",I188&gt;=2.8,"C",I188&gt;=2.5,"D",I188&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K188" s="9" t="str" cm="1">
@@ -8305,7 +8304,7 @@
         <v>2.7</v>
       </c>
       <c r="J189" s="9" t="str" cm="1">
-        <f t="array" ref="J189">_xlfn.IFS(I189&gt;=3.7,"A",I189&gt;=3.3,"B",I189&gt;=2.9,"C",I189&gt;=2.6,"D",I189&lt;=2.5,"E")</f>
+        <f t="array" ref="J189">_xlfn.IFS(I189&gt;=3.7,"A",I189&gt;=3.3,"B",I189&gt;=2.8,"C",I189&gt;=2.5,"D",I189&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K189" s="9" t="str" cm="1">
@@ -8346,7 +8345,7 @@
         <v>2.7</v>
       </c>
       <c r="J190" s="9" t="str" cm="1">
-        <f t="array" ref="J190">_xlfn.IFS(I190&gt;=3.7,"A",I190&gt;=3.3,"B",I190&gt;=2.9,"C",I190&gt;=2.6,"D",I190&lt;=2.5,"E")</f>
+        <f t="array" ref="J190">_xlfn.IFS(I190&gt;=3.7,"A",I190&gt;=3.3,"B",I190&gt;=2.8,"C",I190&gt;=2.5,"D",I190&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K190" s="9" t="str" cm="1">
@@ -8387,7 +8386,7 @@
         <v>2.7</v>
       </c>
       <c r="J191" s="9" t="str" cm="1">
-        <f t="array" ref="J191">_xlfn.IFS(I191&gt;=3.7,"A",I191&gt;=3.3,"B",I191&gt;=2.9,"C",I191&gt;=2.6,"D",I191&lt;=2.5,"E")</f>
+        <f t="array" ref="J191">_xlfn.IFS(I191&gt;=3.7,"A",I191&gt;=3.3,"B",I191&gt;=2.8,"C",I191&gt;=2.5,"D",I191&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K191" s="9" t="str" cm="1">
@@ -8428,7 +8427,7 @@
         <v>2.7</v>
       </c>
       <c r="J192" s="9" t="str" cm="1">
-        <f t="array" ref="J192">_xlfn.IFS(I192&gt;=3.7,"A",I192&gt;=3.3,"B",I192&gt;=2.9,"C",I192&gt;=2.6,"D",I192&lt;=2.5,"E")</f>
+        <f t="array" ref="J192">_xlfn.IFS(I192&gt;=3.7,"A",I192&gt;=3.3,"B",I192&gt;=2.8,"C",I192&gt;=2.5,"D",I192&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K192" s="9" t="str" cm="1">
@@ -8469,7 +8468,7 @@
         <v>2.7</v>
       </c>
       <c r="J193" s="9" t="str" cm="1">
-        <f t="array" ref="J193">_xlfn.IFS(I193&gt;=3.7,"A",I193&gt;=3.3,"B",I193&gt;=2.9,"C",I193&gt;=2.6,"D",I193&lt;=2.5,"E")</f>
+        <f t="array" ref="J193">_xlfn.IFS(I193&gt;=3.7,"A",I193&gt;=3.3,"B",I193&gt;=2.8,"C",I193&gt;=2.5,"D",I193&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K193" s="9" t="str" cm="1">
@@ -8510,7 +8509,7 @@
         <v>2.7</v>
       </c>
       <c r="J194" s="9" t="str" cm="1">
-        <f t="array" ref="J194">_xlfn.IFS(I194&gt;=3.7,"A",I194&gt;=3.3,"B",I194&gt;=2.9,"C",I194&gt;=2.6,"D",I194&lt;=2.5,"E")</f>
+        <f t="array" ref="J194">_xlfn.IFS(I194&gt;=3.7,"A",I194&gt;=3.3,"B",I194&gt;=2.8,"C",I194&gt;=2.5,"D",I194&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K194" s="9" t="str" cm="1">
@@ -8551,7 +8550,7 @@
         <v>2.7</v>
       </c>
       <c r="J195" s="9" t="str" cm="1">
-        <f t="array" ref="J195">_xlfn.IFS(I195&gt;=3.7,"A",I195&gt;=3.3,"B",I195&gt;=2.9,"C",I195&gt;=2.6,"D",I195&lt;=2.5,"E")</f>
+        <f t="array" ref="J195">_xlfn.IFS(I195&gt;=3.7,"A",I195&gt;=3.3,"B",I195&gt;=2.8,"C",I195&gt;=2.5,"D",I195&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K195" s="9" t="str" cm="1">
@@ -8592,7 +8591,7 @@
         <v>2.7</v>
       </c>
       <c r="J196" s="9" t="str" cm="1">
-        <f t="array" ref="J196">_xlfn.IFS(I196&gt;=3.7,"A",I196&gt;=3.3,"B",I196&gt;=2.9,"C",I196&gt;=2.6,"D",I196&lt;=2.5,"E")</f>
+        <f t="array" ref="J196">_xlfn.IFS(I196&gt;=3.7,"A",I196&gt;=3.3,"B",I196&gt;=2.8,"C",I196&gt;=2.5,"D",I196&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K196" s="9" t="str" cm="1">
@@ -8633,7 +8632,7 @@
         <v>2.7</v>
       </c>
       <c r="J197" s="9" t="str" cm="1">
-        <f t="array" ref="J197">_xlfn.IFS(I197&gt;=3.7,"A",I197&gt;=3.3,"B",I197&gt;=2.9,"C",I197&gt;=2.6,"D",I197&lt;=2.5,"E")</f>
+        <f t="array" ref="J197">_xlfn.IFS(I197&gt;=3.7,"A",I197&gt;=3.3,"B",I197&gt;=2.8,"C",I197&gt;=2.5,"D",I197&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K197" s="9" t="str" cm="1">
@@ -8674,7 +8673,7 @@
         <v>2.6</v>
       </c>
       <c r="J198" s="9" t="str" cm="1">
-        <f t="array" ref="J198">_xlfn.IFS(I198&gt;=3.7,"A",I198&gt;=3.3,"B",I198&gt;=2.9,"C",I198&gt;=2.6,"D",I198&lt;=2.5,"E")</f>
+        <f t="array" ref="J198">_xlfn.IFS(I198&gt;=3.7,"A",I198&gt;=3.3,"B",I198&gt;=2.8,"C",I198&gt;=2.5,"D",I198&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K198" s="9" t="str" cm="1">
@@ -8715,7 +8714,7 @@
         <v>2.6</v>
       </c>
       <c r="J199" s="9" t="str" cm="1">
-        <f t="array" ref="J199">_xlfn.IFS(I199&gt;=3.7,"A",I199&gt;=3.3,"B",I199&gt;=2.9,"C",I199&gt;=2.6,"D",I199&lt;=2.5,"E")</f>
+        <f t="array" ref="J199">_xlfn.IFS(I199&gt;=3.7,"A",I199&gt;=3.3,"B",I199&gt;=2.8,"C",I199&gt;=2.5,"D",I199&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K199" s="9" t="str" cm="1">
@@ -8756,7 +8755,7 @@
         <v>2.6</v>
       </c>
       <c r="J200" s="9" t="str" cm="1">
-        <f t="array" ref="J200">_xlfn.IFS(I200&gt;=3.7,"A",I200&gt;=3.3,"B",I200&gt;=2.9,"C",I200&gt;=2.6,"D",I200&lt;=2.5,"E")</f>
+        <f t="array" ref="J200">_xlfn.IFS(I200&gt;=3.7,"A",I200&gt;=3.3,"B",I200&gt;=2.8,"C",I200&gt;=2.5,"D",I200&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K200" s="9" t="str" cm="1">
@@ -8797,7 +8796,7 @@
         <v>2.6</v>
       </c>
       <c r="J201" s="9" t="str" cm="1">
-        <f t="array" ref="J201">_xlfn.IFS(I201&gt;=3.7,"A",I201&gt;=3.3,"B",I201&gt;=2.9,"C",I201&gt;=2.6,"D",I201&lt;=2.5,"E")</f>
+        <f t="array" ref="J201">_xlfn.IFS(I201&gt;=3.7,"A",I201&gt;=3.3,"B",I201&gt;=2.8,"C",I201&gt;=2.5,"D",I201&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K201" s="9" t="str" cm="1">
@@ -8838,7 +8837,7 @@
         <v>2.6</v>
       </c>
       <c r="J202" s="9" t="str" cm="1">
-        <f t="array" ref="J202">_xlfn.IFS(I202&gt;=3.7,"A",I202&gt;=3.3,"B",I202&gt;=2.9,"C",I202&gt;=2.6,"D",I202&lt;=2.5,"E")</f>
+        <f t="array" ref="J202">_xlfn.IFS(I202&gt;=3.7,"A",I202&gt;=3.3,"B",I202&gt;=2.8,"C",I202&gt;=2.5,"D",I202&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K202" s="9" t="str" cm="1">
@@ -8879,7 +8878,7 @@
         <v>2.6</v>
       </c>
       <c r="J203" s="9" t="str" cm="1">
-        <f t="array" ref="J203">_xlfn.IFS(I203&gt;=3.7,"A",I203&gt;=3.3,"B",I203&gt;=2.9,"C",I203&gt;=2.6,"D",I203&lt;=2.5,"E")</f>
+        <f t="array" ref="J203">_xlfn.IFS(I203&gt;=3.7,"A",I203&gt;=3.3,"B",I203&gt;=2.8,"C",I203&gt;=2.5,"D",I203&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K203" s="9" t="str" cm="1">
@@ -8920,7 +8919,7 @@
         <v>2.6</v>
       </c>
       <c r="J204" s="9" t="str" cm="1">
-        <f t="array" ref="J204">_xlfn.IFS(I204&gt;=3.7,"A",I204&gt;=3.3,"B",I204&gt;=2.9,"C",I204&gt;=2.6,"D",I204&lt;=2.5,"E")</f>
+        <f t="array" ref="J204">_xlfn.IFS(I204&gt;=3.7,"A",I204&gt;=3.3,"B",I204&gt;=2.8,"C",I204&gt;=2.5,"D",I204&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K204" s="9" t="str" cm="1">
@@ -8961,7 +8960,7 @@
         <v>2.6</v>
       </c>
       <c r="J205" s="9" t="str" cm="1">
-        <f t="array" ref="J205">_xlfn.IFS(I205&gt;=3.7,"A",I205&gt;=3.3,"B",I205&gt;=2.9,"C",I205&gt;=2.6,"D",I205&lt;=2.5,"E")</f>
+        <f t="array" ref="J205">_xlfn.IFS(I205&gt;=3.7,"A",I205&gt;=3.3,"B",I205&gt;=2.8,"C",I205&gt;=2.5,"D",I205&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K205" s="9" t="str" cm="1">
@@ -9002,7 +9001,7 @@
         <v>2.6</v>
       </c>
       <c r="J206" s="9" t="str" cm="1">
-        <f t="array" ref="J206">_xlfn.IFS(I206&gt;=3.7,"A",I206&gt;=3.3,"B",I206&gt;=2.9,"C",I206&gt;=2.6,"D",I206&lt;=2.5,"E")</f>
+        <f t="array" ref="J206">_xlfn.IFS(I206&gt;=3.7,"A",I206&gt;=3.3,"B",I206&gt;=2.8,"C",I206&gt;=2.5,"D",I206&lt;=2.4,"E")</f>
         <v>D</v>
       </c>
       <c r="K206" s="9" t="str" cm="1">
@@ -9043,8 +9042,8 @@
         <v>2.5</v>
       </c>
       <c r="J207" s="9" t="str" cm="1">
-        <f t="array" ref="J207">_xlfn.IFS(I207&gt;=3.7,"A",I207&gt;=3.3,"B",I207&gt;=2.9,"C",I207&gt;=2.6,"D",I207&lt;=2.5,"E")</f>
-        <v>E</v>
+        <f t="array" ref="J207">_xlfn.IFS(I207&gt;=3.7,"A",I207&gt;=3.3,"B",I207&gt;=2.8,"C",I207&gt;=2.5,"D",I207&lt;=2.4,"E")</f>
+        <v>D</v>
       </c>
       <c r="K207" s="9" t="str" cm="1">
         <f t="array" ref="K207">_xlfn.IFS(J207="A","LULUS",J207="B","LULUS",J207="C","LULUS",J207="D","TIDAK LULUS",J207="E","TIDAK LULUS")</f>
@@ -9084,8 +9083,8 @@
         <v>2.5</v>
       </c>
       <c r="J208" s="9" t="str" cm="1">
-        <f t="array" ref="J208">_xlfn.IFS(I208&gt;=3.7,"A",I208&gt;=3.3,"B",I208&gt;=2.9,"C",I208&gt;=2.6,"D",I208&lt;=2.5,"E")</f>
-        <v>E</v>
+        <f t="array" ref="J208">_xlfn.IFS(I208&gt;=3.7,"A",I208&gt;=3.3,"B",I208&gt;=2.8,"C",I208&gt;=2.5,"D",I208&lt;=2.4,"E")</f>
+        <v>D</v>
       </c>
       <c r="K208" s="9" t="str" cm="1">
         <f t="array" ref="K208">_xlfn.IFS(J208="A","LULUS",J208="B","LULUS",J208="C","LULUS",J208="D","TIDAK LULUS",J208="E","TIDAK LULUS")</f>
@@ -9125,8 +9124,8 @@
         <v>2.5</v>
       </c>
       <c r="J209" s="9" t="str" cm="1">
-        <f t="array" ref="J209">_xlfn.IFS(I209&gt;=3.7,"A",I209&gt;=3.3,"B",I209&gt;=2.9,"C",I209&gt;=2.6,"D",I209&lt;=2.5,"E")</f>
-        <v>E</v>
+        <f t="array" ref="J209">_xlfn.IFS(I209&gt;=3.7,"A",I209&gt;=3.3,"B",I209&gt;=2.8,"C",I209&gt;=2.5,"D",I209&lt;=2.4,"E")</f>
+        <v>D</v>
       </c>
       <c r="K209" s="9" t="str" cm="1">
         <f t="array" ref="K209">_xlfn.IFS(J209="A","LULUS",J209="B","LULUS",J209="C","LULUS",J209="D","TIDAK LULUS",J209="E","TIDAK LULUS")</f>
@@ -9166,8 +9165,8 @@
         <v>2.5</v>
       </c>
       <c r="J210" s="9" t="str" cm="1">
-        <f t="array" ref="J210">_xlfn.IFS(I210&gt;=3.7,"A",I210&gt;=3.3,"B",I210&gt;=2.9,"C",I210&gt;=2.6,"D",I210&lt;=2.5,"E")</f>
-        <v>E</v>
+        <f t="array" ref="J210">_xlfn.IFS(I210&gt;=3.7,"A",I210&gt;=3.3,"B",I210&gt;=2.8,"C",I210&gt;=2.5,"D",I210&lt;=2.4,"E")</f>
+        <v>D</v>
       </c>
       <c r="K210" s="9" t="str" cm="1">
         <f t="array" ref="K210">_xlfn.IFS(J210="A","LULUS",J210="B","LULUS",J210="C","LULUS",J210="D","TIDAK LULUS",J210="E","TIDAK LULUS")</f>
@@ -9207,8 +9206,8 @@
         <v>2.5</v>
       </c>
       <c r="J211" s="9" t="str" cm="1">
-        <f t="array" ref="J211">_xlfn.IFS(I211&gt;=3.7,"A",I211&gt;=3.3,"B",I211&gt;=2.9,"C",I211&gt;=2.6,"D",I211&lt;=2.5,"E")</f>
-        <v>E</v>
+        <f t="array" ref="J211">_xlfn.IFS(I211&gt;=3.7,"A",I211&gt;=3.3,"B",I211&gt;=2.8,"C",I211&gt;=2.5,"D",I211&lt;=2.4,"E")</f>
+        <v>D</v>
       </c>
       <c r="K211" s="9" t="str" cm="1">
         <f t="array" ref="K211">_xlfn.IFS(J211="A","LULUS",J211="B","LULUS",J211="C","LULUS",J211="D","TIDAK LULUS",J211="E","TIDAK LULUS")</f>
@@ -9248,8 +9247,8 @@
         <v>2.5</v>
       </c>
       <c r="J212" s="9" t="str" cm="1">
-        <f t="array" ref="J212">_xlfn.IFS(I212&gt;=3.7,"A",I212&gt;=3.3,"B",I212&gt;=2.9,"C",I212&gt;=2.6,"D",I212&lt;=2.5,"E")</f>
-        <v>E</v>
+        <f t="array" ref="J212">_xlfn.IFS(I212&gt;=3.7,"A",I212&gt;=3.3,"B",I212&gt;=2.8,"C",I212&gt;=2.5,"D",I212&lt;=2.4,"E")</f>
+        <v>D</v>
       </c>
       <c r="K212" s="9" t="str" cm="1">
         <f t="array" ref="K212">_xlfn.IFS(J212="A","LULUS",J212="B","LULUS",J212="C","LULUS",J212="D","TIDAK LULUS",J212="E","TIDAK LULUS")</f>
@@ -9289,8 +9288,8 @@
         <v>2.5</v>
       </c>
       <c r="J213" s="9" t="str" cm="1">
-        <f t="array" ref="J213">_xlfn.IFS(I213&gt;=3.7,"A",I213&gt;=3.3,"B",I213&gt;=2.9,"C",I213&gt;=2.6,"D",I213&lt;=2.5,"E")</f>
-        <v>E</v>
+        <f t="array" ref="J213">_xlfn.IFS(I213&gt;=3.7,"A",I213&gt;=3.3,"B",I213&gt;=2.8,"C",I213&gt;=2.5,"D",I213&lt;=2.4,"E")</f>
+        <v>D</v>
       </c>
       <c r="K213" s="9" t="str" cm="1">
         <f t="array" ref="K213">_xlfn.IFS(J213="A","LULUS",J213="B","LULUS",J213="C","LULUS",J213="D","TIDAK LULUS",J213="E","TIDAK LULUS")</f>
@@ -9330,8 +9329,8 @@
         <v>2.5</v>
       </c>
       <c r="J214" s="9" t="str" cm="1">
-        <f t="array" ref="J214">_xlfn.IFS(I214&gt;=3.7,"A",I214&gt;=3.3,"B",I214&gt;=2.9,"C",I214&gt;=2.6,"D",I214&lt;=2.5,"E")</f>
-        <v>E</v>
+        <f t="array" ref="J214">_xlfn.IFS(I214&gt;=3.7,"A",I214&gt;=3.3,"B",I214&gt;=2.8,"C",I214&gt;=2.5,"D",I214&lt;=2.4,"E")</f>
+        <v>D</v>
       </c>
       <c r="K214" s="9" t="str" cm="1">
         <f t="array" ref="K214">_xlfn.IFS(J214="A","LULUS",J214="B","LULUS",J214="C","LULUS",J214="D","TIDAK LULUS",J214="E","TIDAK LULUS")</f>
@@ -9371,8 +9370,8 @@
         <v>2.5</v>
       </c>
       <c r="J215" s="9" t="str" cm="1">
-        <f t="array" ref="J215">_xlfn.IFS(I215&gt;=3.7,"A",I215&gt;=3.3,"B",I215&gt;=2.9,"C",I215&gt;=2.6,"D",I215&lt;=2.5,"E")</f>
-        <v>E</v>
+        <f t="array" ref="J215">_xlfn.IFS(I215&gt;=3.7,"A",I215&gt;=3.3,"B",I215&gt;=2.8,"C",I215&gt;=2.5,"D",I215&lt;=2.4,"E")</f>
+        <v>D</v>
       </c>
       <c r="K215" s="9" t="str" cm="1">
         <f t="array" ref="K215">_xlfn.IFS(J215="A","LULUS",J215="B","LULUS",J215="C","LULUS",J215="D","TIDAK LULUS",J215="E","TIDAK LULUS")</f>
@@ -9412,7 +9411,7 @@
         <v>2.4</v>
       </c>
       <c r="J216" s="9" t="str" cm="1">
-        <f t="array" ref="J216">_xlfn.IFS(I216&gt;=3.7,"A",I216&gt;=3.3,"B",I216&gt;=2.9,"C",I216&gt;=2.6,"D",I216&lt;=2.5,"E")</f>
+        <f t="array" ref="J216">_xlfn.IFS(I216&gt;=3.7,"A",I216&gt;=3.3,"B",I216&gt;=2.8,"C",I216&gt;=2.5,"D",I216&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K216" s="9" t="str" cm="1">
@@ -9453,7 +9452,7 @@
         <v>2.4</v>
       </c>
       <c r="J217" s="9" t="str" cm="1">
-        <f t="array" ref="J217">_xlfn.IFS(I217&gt;=3.7,"A",I217&gt;=3.3,"B",I217&gt;=2.9,"C",I217&gt;=2.6,"D",I217&lt;=2.5,"E")</f>
+        <f t="array" ref="J217">_xlfn.IFS(I217&gt;=3.7,"A",I217&gt;=3.3,"B",I217&gt;=2.8,"C",I217&gt;=2.5,"D",I217&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K217" s="9" t="str" cm="1">
@@ -9494,7 +9493,7 @@
         <v>2.4</v>
       </c>
       <c r="J218" s="9" t="str" cm="1">
-        <f t="array" ref="J218">_xlfn.IFS(I218&gt;=3.7,"A",I218&gt;=3.3,"B",I218&gt;=2.9,"C",I218&gt;=2.6,"D",I218&lt;=2.5,"E")</f>
+        <f t="array" ref="J218">_xlfn.IFS(I218&gt;=3.7,"A",I218&gt;=3.3,"B",I218&gt;=2.8,"C",I218&gt;=2.5,"D",I218&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K218" s="9" t="str" cm="1">
@@ -9535,7 +9534,7 @@
         <v>2.4</v>
       </c>
       <c r="J219" s="9" t="str" cm="1">
-        <f t="array" ref="J219">_xlfn.IFS(I219&gt;=3.7,"A",I219&gt;=3.3,"B",I219&gt;=2.9,"C",I219&gt;=2.6,"D",I219&lt;=2.5,"E")</f>
+        <f t="array" ref="J219">_xlfn.IFS(I219&gt;=3.7,"A",I219&gt;=3.3,"B",I219&gt;=2.8,"C",I219&gt;=2.5,"D",I219&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K219" s="9" t="str" cm="1">
@@ -9576,7 +9575,7 @@
         <v>2.4</v>
       </c>
       <c r="J220" s="9" t="str" cm="1">
-        <f t="array" ref="J220">_xlfn.IFS(I220&gt;=3.7,"A",I220&gt;=3.3,"B",I220&gt;=2.9,"C",I220&gt;=2.6,"D",I220&lt;=2.5,"E")</f>
+        <f t="array" ref="J220">_xlfn.IFS(I220&gt;=3.7,"A",I220&gt;=3.3,"B",I220&gt;=2.8,"C",I220&gt;=2.5,"D",I220&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K220" s="9" t="str" cm="1">
@@ -9617,7 +9616,7 @@
         <v>2.4</v>
       </c>
       <c r="J221" s="9" t="str" cm="1">
-        <f t="array" ref="J221">_xlfn.IFS(I221&gt;=3.7,"A",I221&gt;=3.3,"B",I221&gt;=2.9,"C",I221&gt;=2.6,"D",I221&lt;=2.5,"E")</f>
+        <f t="array" ref="J221">_xlfn.IFS(I221&gt;=3.7,"A",I221&gt;=3.3,"B",I221&gt;=2.8,"C",I221&gt;=2.5,"D",I221&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K221" s="9" t="str" cm="1">
@@ -9658,7 +9657,7 @@
         <v>2.4</v>
       </c>
       <c r="J222" s="9" t="str" cm="1">
-        <f t="array" ref="J222">_xlfn.IFS(I222&gt;=3.7,"A",I222&gt;=3.3,"B",I222&gt;=2.9,"C",I222&gt;=2.6,"D",I222&lt;=2.5,"E")</f>
+        <f t="array" ref="J222">_xlfn.IFS(I222&gt;=3.7,"A",I222&gt;=3.3,"B",I222&gt;=2.8,"C",I222&gt;=2.5,"D",I222&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K222" s="9" t="str" cm="1">
@@ -9699,7 +9698,7 @@
         <v>2.4</v>
       </c>
       <c r="J223" s="9" t="str" cm="1">
-        <f t="array" ref="J223">_xlfn.IFS(I223&gt;=3.7,"A",I223&gt;=3.3,"B",I223&gt;=2.9,"C",I223&gt;=2.6,"D",I223&lt;=2.5,"E")</f>
+        <f t="array" ref="J223">_xlfn.IFS(I223&gt;=3.7,"A",I223&gt;=3.3,"B",I223&gt;=2.8,"C",I223&gt;=2.5,"D",I223&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K223" s="9" t="str" cm="1">
@@ -9740,7 +9739,7 @@
         <v>2.4</v>
       </c>
       <c r="J224" s="9" t="str" cm="1">
-        <f t="array" ref="J224">_xlfn.IFS(I224&gt;=3.7,"A",I224&gt;=3.3,"B",I224&gt;=2.9,"C",I224&gt;=2.6,"D",I224&lt;=2.5,"E")</f>
+        <f t="array" ref="J224">_xlfn.IFS(I224&gt;=3.7,"A",I224&gt;=3.3,"B",I224&gt;=2.8,"C",I224&gt;=2.5,"D",I224&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K224" s="9" t="str" cm="1">
@@ -9781,7 +9780,7 @@
         <v>2.4</v>
       </c>
       <c r="J225" s="9" t="str" cm="1">
-        <f t="array" ref="J225">_xlfn.IFS(I225&gt;=3.7,"A",I225&gt;=3.3,"B",I225&gt;=2.9,"C",I225&gt;=2.6,"D",I225&lt;=2.5,"E")</f>
+        <f t="array" ref="J225">_xlfn.IFS(I225&gt;=3.7,"A",I225&gt;=3.3,"B",I225&gt;=2.8,"C",I225&gt;=2.5,"D",I225&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K225" s="9" t="str" cm="1">
@@ -9822,7 +9821,7 @@
         <v>2.4</v>
       </c>
       <c r="J226" s="9" t="str" cm="1">
-        <f t="array" ref="J226">_xlfn.IFS(I226&gt;=3.7,"A",I226&gt;=3.3,"B",I226&gt;=2.9,"C",I226&gt;=2.6,"D",I226&lt;=2.5,"E")</f>
+        <f t="array" ref="J226">_xlfn.IFS(I226&gt;=3.7,"A",I226&gt;=3.3,"B",I226&gt;=2.8,"C",I226&gt;=2.5,"D",I226&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K226" s="9" t="str" cm="1">
@@ -9863,7 +9862,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="J227" s="9" t="str" cm="1">
-        <f t="array" ref="J227">_xlfn.IFS(I227&gt;=3.7,"A",I227&gt;=3.3,"B",I227&gt;=2.9,"C",I227&gt;=2.6,"D",I227&lt;=2.5,"E")</f>
+        <f t="array" ref="J227">_xlfn.IFS(I227&gt;=3.7,"A",I227&gt;=3.3,"B",I227&gt;=2.8,"C",I227&gt;=2.5,"D",I227&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K227" s="9" t="str" cm="1">
@@ -9904,7 +9903,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="J228" s="9" t="str" cm="1">
-        <f t="array" ref="J228">_xlfn.IFS(I228&gt;=3.7,"A",I228&gt;=3.3,"B",I228&gt;=2.9,"C",I228&gt;=2.6,"D",I228&lt;=2.5,"E")</f>
+        <f t="array" ref="J228">_xlfn.IFS(I228&gt;=3.7,"A",I228&gt;=3.3,"B",I228&gt;=2.8,"C",I228&gt;=2.5,"D",I228&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K228" s="9" t="str" cm="1">
@@ -9945,7 +9944,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="J229" s="9" t="str" cm="1">
-        <f t="array" ref="J229">_xlfn.IFS(I229&gt;=3.7,"A",I229&gt;=3.3,"B",I229&gt;=2.9,"C",I229&gt;=2.6,"D",I229&lt;=2.5,"E")</f>
+        <f t="array" ref="J229">_xlfn.IFS(I229&gt;=3.7,"A",I229&gt;=3.3,"B",I229&gt;=2.8,"C",I229&gt;=2.5,"D",I229&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K229" s="9" t="str" cm="1">
@@ -9986,7 +9985,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="J230" s="9" t="str" cm="1">
-        <f t="array" ref="J230">_xlfn.IFS(I230&gt;=3.7,"A",I230&gt;=3.3,"B",I230&gt;=2.9,"C",I230&gt;=2.6,"D",I230&lt;=2.5,"E")</f>
+        <f t="array" ref="J230">_xlfn.IFS(I230&gt;=3.7,"A",I230&gt;=3.3,"B",I230&gt;=2.8,"C",I230&gt;=2.5,"D",I230&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K230" s="9" t="str" cm="1">
@@ -10027,7 +10026,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="J231" s="9" t="str" cm="1">
-        <f t="array" ref="J231">_xlfn.IFS(I231&gt;=3.7,"A",I231&gt;=3.3,"B",I231&gt;=2.9,"C",I231&gt;=2.6,"D",I231&lt;=2.5,"E")</f>
+        <f t="array" ref="J231">_xlfn.IFS(I231&gt;=3.7,"A",I231&gt;=3.3,"B",I231&gt;=2.8,"C",I231&gt;=2.5,"D",I231&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K231" s="9" t="str" cm="1">
@@ -10068,7 +10067,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="J232" s="9" t="str" cm="1">
-        <f t="array" ref="J232">_xlfn.IFS(I232&gt;=3.7,"A",I232&gt;=3.3,"B",I232&gt;=2.9,"C",I232&gt;=2.6,"D",I232&lt;=2.5,"E")</f>
+        <f t="array" ref="J232">_xlfn.IFS(I232&gt;=3.7,"A",I232&gt;=3.3,"B",I232&gt;=2.8,"C",I232&gt;=2.5,"D",I232&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K232" s="9" t="str" cm="1">
@@ -10109,7 +10108,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="J233" s="9" t="str" cm="1">
-        <f t="array" ref="J233">_xlfn.IFS(I233&gt;=3.7,"A",I233&gt;=3.3,"B",I233&gt;=2.9,"C",I233&gt;=2.6,"D",I233&lt;=2.5,"E")</f>
+        <f t="array" ref="J233">_xlfn.IFS(I233&gt;=3.7,"A",I233&gt;=3.3,"B",I233&gt;=2.8,"C",I233&gt;=2.5,"D",I233&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K233" s="9" t="str" cm="1">
@@ -10150,7 +10149,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="J234" s="9" t="str" cm="1">
-        <f t="array" ref="J234">_xlfn.IFS(I234&gt;=3.7,"A",I234&gt;=3.3,"B",I234&gt;=2.9,"C",I234&gt;=2.6,"D",I234&lt;=2.5,"E")</f>
+        <f t="array" ref="J234">_xlfn.IFS(I234&gt;=3.7,"A",I234&gt;=3.3,"B",I234&gt;=2.8,"C",I234&gt;=2.5,"D",I234&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K234" s="9" t="str" cm="1">
@@ -10191,7 +10190,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="J235" s="9" t="str" cm="1">
-        <f t="array" ref="J235">_xlfn.IFS(I235&gt;=3.7,"A",I235&gt;=3.3,"B",I235&gt;=2.9,"C",I235&gt;=2.6,"D",I235&lt;=2.5,"E")</f>
+        <f t="array" ref="J235">_xlfn.IFS(I235&gt;=3.7,"A",I235&gt;=3.3,"B",I235&gt;=2.8,"C",I235&gt;=2.5,"D",I235&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K235" s="9" t="str" cm="1">
@@ -10232,7 +10231,7 @@
         <v>2.1</v>
       </c>
       <c r="J236" s="9" t="str" cm="1">
-        <f t="array" ref="J236">_xlfn.IFS(I236&gt;=3.7,"A",I236&gt;=3.3,"B",I236&gt;=2.9,"C",I236&gt;=2.6,"D",I236&lt;=2.5,"E")</f>
+        <f t="array" ref="J236">_xlfn.IFS(I236&gt;=3.7,"A",I236&gt;=3.3,"B",I236&gt;=2.8,"C",I236&gt;=2.5,"D",I236&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K236" s="9" t="str" cm="1">
@@ -10273,7 +10272,7 @@
         <v>2.1</v>
       </c>
       <c r="J237" s="9" t="str" cm="1">
-        <f t="array" ref="J237">_xlfn.IFS(I237&gt;=3.7,"A",I237&gt;=3.3,"B",I237&gt;=2.9,"C",I237&gt;=2.6,"D",I237&lt;=2.5,"E")</f>
+        <f t="array" ref="J237">_xlfn.IFS(I237&gt;=3.7,"A",I237&gt;=3.3,"B",I237&gt;=2.8,"C",I237&gt;=2.5,"D",I237&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K237" s="9" t="str" cm="1">
@@ -10314,7 +10313,7 @@
         <v>2.1</v>
       </c>
       <c r="J238" s="9" t="str" cm="1">
-        <f t="array" ref="J238">_xlfn.IFS(I238&gt;=3.7,"A",I238&gt;=3.3,"B",I238&gt;=2.9,"C",I238&gt;=2.6,"D",I238&lt;=2.5,"E")</f>
+        <f t="array" ref="J238">_xlfn.IFS(I238&gt;=3.7,"A",I238&gt;=3.3,"B",I238&gt;=2.8,"C",I238&gt;=2.5,"D",I238&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K238" s="9" t="str" cm="1">
@@ -10355,7 +10354,7 @@
         <v>2.1</v>
       </c>
       <c r="J239" s="9" t="str" cm="1">
-        <f t="array" ref="J239">_xlfn.IFS(I239&gt;=3.7,"A",I239&gt;=3.3,"B",I239&gt;=2.9,"C",I239&gt;=2.6,"D",I239&lt;=2.5,"E")</f>
+        <f t="array" ref="J239">_xlfn.IFS(I239&gt;=3.7,"A",I239&gt;=3.3,"B",I239&gt;=2.8,"C",I239&gt;=2.5,"D",I239&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K239" s="9" t="str" cm="1">
@@ -10396,7 +10395,7 @@
         <v>2</v>
       </c>
       <c r="J240" s="9" t="str" cm="1">
-        <f t="array" ref="J240">_xlfn.IFS(I240&gt;=3.7,"A",I240&gt;=3.3,"B",I240&gt;=2.9,"C",I240&gt;=2.6,"D",I240&lt;=2.5,"E")</f>
+        <f t="array" ref="J240">_xlfn.IFS(I240&gt;=3.7,"A",I240&gt;=3.3,"B",I240&gt;=2.8,"C",I240&gt;=2.5,"D",I240&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K240" s="9" t="str" cm="1">
@@ -10437,7 +10436,7 @@
         <v>2</v>
       </c>
       <c r="J241" s="9" t="str" cm="1">
-        <f t="array" ref="J241">_xlfn.IFS(I241&gt;=3.7,"A",I241&gt;=3.3,"B",I241&gt;=2.9,"C",I241&gt;=2.6,"D",I241&lt;=2.5,"E")</f>
+        <f t="array" ref="J241">_xlfn.IFS(I241&gt;=3.7,"A",I241&gt;=3.3,"B",I241&gt;=2.8,"C",I241&gt;=2.5,"D",I241&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K241" s="9" t="str" cm="1">
@@ -10478,7 +10477,7 @@
         <v>2</v>
       </c>
       <c r="J242" s="9" t="str" cm="1">
-        <f t="array" ref="J242">_xlfn.IFS(I242&gt;=3.7,"A",I242&gt;=3.3,"B",I242&gt;=2.9,"C",I242&gt;=2.6,"D",I242&lt;=2.5,"E")</f>
+        <f t="array" ref="J242">_xlfn.IFS(I242&gt;=3.7,"A",I242&gt;=3.3,"B",I242&gt;=2.8,"C",I242&gt;=2.5,"D",I242&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K242" s="9" t="str" cm="1">
@@ -10519,7 +10518,7 @@
         <v>1.9</v>
       </c>
       <c r="J243" s="9" t="str" cm="1">
-        <f t="array" ref="J243">_xlfn.IFS(I243&gt;=3.7,"A",I243&gt;=3.3,"B",I243&gt;=2.9,"C",I243&gt;=2.6,"D",I243&lt;=2.5,"E")</f>
+        <f t="array" ref="J243">_xlfn.IFS(I243&gt;=3.7,"A",I243&gt;=3.3,"B",I243&gt;=2.8,"C",I243&gt;=2.5,"D",I243&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K243" s="9" t="str" cm="1">
@@ -10560,7 +10559,7 @@
         <v>1.9</v>
       </c>
       <c r="J244" s="9" t="str" cm="1">
-        <f t="array" ref="J244">_xlfn.IFS(I244&gt;=3.7,"A",I244&gt;=3.3,"B",I244&gt;=2.9,"C",I244&gt;=2.6,"D",I244&lt;=2.5,"E")</f>
+        <f t="array" ref="J244">_xlfn.IFS(I244&gt;=3.7,"A",I244&gt;=3.3,"B",I244&gt;=2.8,"C",I244&gt;=2.5,"D",I244&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K244" s="9" t="str" cm="1">
@@ -10601,7 +10600,7 @@
         <v>1.8</v>
       </c>
       <c r="J245" s="9" t="str" cm="1">
-        <f t="array" ref="J245">_xlfn.IFS(I245&gt;=3.7,"A",I245&gt;=3.3,"B",I245&gt;=2.9,"C",I245&gt;=2.6,"D",I245&lt;=2.5,"E")</f>
+        <f t="array" ref="J245">_xlfn.IFS(I245&gt;=3.7,"A",I245&gt;=3.3,"B",I245&gt;=2.8,"C",I245&gt;=2.5,"D",I245&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K245" s="9" t="str" cm="1">
@@ -10642,7 +10641,7 @@
         <v>1.8</v>
       </c>
       <c r="J246" s="9" t="str" cm="1">
-        <f t="array" ref="J246">_xlfn.IFS(I246&gt;=3.7,"A",I246&gt;=3.3,"B",I246&gt;=2.9,"C",I246&gt;=2.6,"D",I246&lt;=2.5,"E")</f>
+        <f t="array" ref="J246">_xlfn.IFS(I246&gt;=3.7,"A",I246&gt;=3.3,"B",I246&gt;=2.8,"C",I246&gt;=2.5,"D",I246&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K246" s="9" t="str" cm="1">
@@ -10683,7 +10682,7 @@
         <v>1.8</v>
       </c>
       <c r="J247" s="9" t="str" cm="1">
-        <f t="array" ref="J247">_xlfn.IFS(I247&gt;=3.7,"A",I247&gt;=3.3,"B",I247&gt;=2.9,"C",I247&gt;=2.6,"D",I247&lt;=2.5,"E")</f>
+        <f t="array" ref="J247">_xlfn.IFS(I247&gt;=3.7,"A",I247&gt;=3.3,"B",I247&gt;=2.8,"C",I247&gt;=2.5,"D",I247&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K247" s="9" t="str" cm="1">
@@ -10724,7 +10723,7 @@
         <v>1.7</v>
       </c>
       <c r="J248" s="9" t="str" cm="1">
-        <f t="array" ref="J248">_xlfn.IFS(I248&gt;=3.7,"A",I248&gt;=3.3,"B",I248&gt;=2.9,"C",I248&gt;=2.6,"D",I248&lt;=2.5,"E")</f>
+        <f t="array" ref="J248">_xlfn.IFS(I248&gt;=3.7,"A",I248&gt;=3.3,"B",I248&gt;=2.8,"C",I248&gt;=2.5,"D",I248&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K248" s="9" t="str" cm="1">
@@ -10765,7 +10764,7 @@
         <v>1.7</v>
       </c>
       <c r="J249" s="9" t="str" cm="1">
-        <f t="array" ref="J249">_xlfn.IFS(I249&gt;=3.7,"A",I249&gt;=3.3,"B",I249&gt;=2.9,"C",I249&gt;=2.6,"D",I249&lt;=2.5,"E")</f>
+        <f t="array" ref="J249">_xlfn.IFS(I249&gt;=3.7,"A",I249&gt;=3.3,"B",I249&gt;=2.8,"C",I249&gt;=2.5,"D",I249&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K249" s="9" t="str" cm="1">
@@ -10806,7 +10805,7 @@
         <v>1.6</v>
       </c>
       <c r="J250" s="9" t="str" cm="1">
-        <f t="array" ref="J250">_xlfn.IFS(I250&gt;=3.7,"A",I250&gt;=3.3,"B",I250&gt;=2.9,"C",I250&gt;=2.6,"D",I250&lt;=2.5,"E")</f>
+        <f t="array" ref="J250">_xlfn.IFS(I250&gt;=3.7,"A",I250&gt;=3.3,"B",I250&gt;=2.8,"C",I250&gt;=2.5,"D",I250&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K250" s="9" t="str" cm="1">
@@ -10847,7 +10846,7 @@
         <v>1.6</v>
       </c>
       <c r="J251" s="9" t="str" cm="1">
-        <f t="array" ref="J251">_xlfn.IFS(I251&gt;=3.7,"A",I251&gt;=3.3,"B",I251&gt;=2.9,"C",I251&gt;=2.6,"D",I251&lt;=2.5,"E")</f>
+        <f t="array" ref="J251">_xlfn.IFS(I251&gt;=3.7,"A",I251&gt;=3.3,"B",I251&gt;=2.8,"C",I251&gt;=2.5,"D",I251&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K251" s="9" t="str" cm="1">
@@ -10888,7 +10887,7 @@
         <v>1.6</v>
       </c>
       <c r="J252" s="9" t="str" cm="1">
-        <f t="array" ref="J252">_xlfn.IFS(I252&gt;=3.7,"A",I252&gt;=3.3,"B",I252&gt;=2.9,"C",I252&gt;=2.6,"D",I252&lt;=2.5,"E")</f>
+        <f t="array" ref="J252">_xlfn.IFS(I252&gt;=3.7,"A",I252&gt;=3.3,"B",I252&gt;=2.8,"C",I252&gt;=2.5,"D",I252&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K252" s="9" t="str" cm="1">
@@ -10929,7 +10928,7 @@
         <v>1.6</v>
       </c>
       <c r="J253" s="9" t="str" cm="1">
-        <f t="array" ref="J253">_xlfn.IFS(I253&gt;=3.7,"A",I253&gt;=3.3,"B",I253&gt;=2.9,"C",I253&gt;=2.6,"D",I253&lt;=2.5,"E")</f>
+        <f t="array" ref="J253">_xlfn.IFS(I253&gt;=3.7,"A",I253&gt;=3.3,"B",I253&gt;=2.8,"C",I253&gt;=2.5,"D",I253&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K253" s="9" t="str" cm="1">
@@ -10970,7 +10969,7 @@
         <v>1.6</v>
       </c>
       <c r="J254" s="9" t="str" cm="1">
-        <f t="array" ref="J254">_xlfn.IFS(I254&gt;=3.7,"A",I254&gt;=3.3,"B",I254&gt;=2.9,"C",I254&gt;=2.6,"D",I254&lt;=2.5,"E")</f>
+        <f t="array" ref="J254">_xlfn.IFS(I254&gt;=3.7,"A",I254&gt;=3.3,"B",I254&gt;=2.8,"C",I254&gt;=2.5,"D",I254&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K254" s="9" t="str" cm="1">
@@ -11011,7 +11010,7 @@
         <v>1.6</v>
       </c>
       <c r="J255" s="9" t="str" cm="1">
-        <f t="array" ref="J255">_xlfn.IFS(I255&gt;=3.7,"A",I255&gt;=3.3,"B",I255&gt;=2.9,"C",I255&gt;=2.6,"D",I255&lt;=2.5,"E")</f>
+        <f t="array" ref="J255">_xlfn.IFS(I255&gt;=3.7,"A",I255&gt;=3.3,"B",I255&gt;=2.8,"C",I255&gt;=2.5,"D",I255&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K255" s="9" t="str" cm="1">
@@ -11052,7 +11051,7 @@
         <v>1.5</v>
       </c>
       <c r="J256" s="9" t="str" cm="1">
-        <f t="array" ref="J256">_xlfn.IFS(I256&gt;=3.7,"A",I256&gt;=3.3,"B",I256&gt;=2.9,"C",I256&gt;=2.6,"D",I256&lt;=2.5,"E")</f>
+        <f t="array" ref="J256">_xlfn.IFS(I256&gt;=3.7,"A",I256&gt;=3.3,"B",I256&gt;=2.8,"C",I256&gt;=2.5,"D",I256&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K256" s="9" t="str" cm="1">
@@ -11093,7 +11092,7 @@
         <v>1.5</v>
       </c>
       <c r="J257" s="9" t="str" cm="1">
-        <f t="array" ref="J257">_xlfn.IFS(I257&gt;=3.7,"A",I257&gt;=3.3,"B",I257&gt;=2.9,"C",I257&gt;=2.6,"D",I257&lt;=2.5,"E")</f>
+        <f t="array" ref="J257">_xlfn.IFS(I257&gt;=3.7,"A",I257&gt;=3.3,"B",I257&gt;=2.8,"C",I257&gt;=2.5,"D",I257&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K257" s="9" t="str" cm="1">
@@ -11134,7 +11133,7 @@
         <v>1.5</v>
       </c>
       <c r="J258" s="9" t="str" cm="1">
-        <f t="array" ref="J258">_xlfn.IFS(I258&gt;=3.7,"A",I258&gt;=3.3,"B",I258&gt;=2.9,"C",I258&gt;=2.6,"D",I258&lt;=2.5,"E")</f>
+        <f t="array" ref="J258">_xlfn.IFS(I258&gt;=3.7,"A",I258&gt;=3.3,"B",I258&gt;=2.8,"C",I258&gt;=2.5,"D",I258&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K258" s="9" t="str" cm="1">
@@ -11175,7 +11174,7 @@
         <v>1.4</v>
       </c>
       <c r="J259" s="9" t="str" cm="1">
-        <f t="array" ref="J259">_xlfn.IFS(I259&gt;=3.7,"A",I259&gt;=3.3,"B",I259&gt;=2.9,"C",I259&gt;=2.6,"D",I259&lt;=2.5,"E")</f>
+        <f t="array" ref="J259">_xlfn.IFS(I259&gt;=3.7,"A",I259&gt;=3.3,"B",I259&gt;=2.8,"C",I259&gt;=2.5,"D",I259&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K259" s="9" t="str" cm="1">
@@ -11216,7 +11215,7 @@
         <v>1.4</v>
       </c>
       <c r="J260" s="9" t="str" cm="1">
-        <f t="array" ref="J260">_xlfn.IFS(I260&gt;=3.7,"A",I260&gt;=3.3,"B",I260&gt;=2.9,"C",I260&gt;=2.6,"D",I260&lt;=2.5,"E")</f>
+        <f t="array" ref="J260">_xlfn.IFS(I260&gt;=3.7,"A",I260&gt;=3.3,"B",I260&gt;=2.8,"C",I260&gt;=2.5,"D",I260&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K260" s="9" t="str" cm="1">
@@ -11257,7 +11256,7 @@
         <v>1.4</v>
       </c>
       <c r="J261" s="9" t="str" cm="1">
-        <f t="array" ref="J261">_xlfn.IFS(I261&gt;=3.7,"A",I261&gt;=3.3,"B",I261&gt;=2.9,"C",I261&gt;=2.6,"D",I261&lt;=2.5,"E")</f>
+        <f t="array" ref="J261">_xlfn.IFS(I261&gt;=3.7,"A",I261&gt;=3.3,"B",I261&gt;=2.8,"C",I261&gt;=2.5,"D",I261&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K261" s="9" t="str" cm="1">
@@ -11298,7 +11297,7 @@
         <v>1.4</v>
       </c>
       <c r="J262" s="9" t="str" cm="1">
-        <f t="array" ref="J262">_xlfn.IFS(I262&gt;=3.7,"A",I262&gt;=3.3,"B",I262&gt;=2.9,"C",I262&gt;=2.6,"D",I262&lt;=2.5,"E")</f>
+        <f t="array" ref="J262">_xlfn.IFS(I262&gt;=3.7,"A",I262&gt;=3.3,"B",I262&gt;=2.8,"C",I262&gt;=2.5,"D",I262&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K262" s="9" t="str" cm="1">
@@ -11339,7 +11338,7 @@
         <v>1.4</v>
       </c>
       <c r="J263" s="9" t="str" cm="1">
-        <f t="array" ref="J263">_xlfn.IFS(I263&gt;=3.7,"A",I263&gt;=3.3,"B",I263&gt;=2.9,"C",I263&gt;=2.6,"D",I263&lt;=2.5,"E")</f>
+        <f t="array" ref="J263">_xlfn.IFS(I263&gt;=3.7,"A",I263&gt;=3.3,"B",I263&gt;=2.8,"C",I263&gt;=2.5,"D",I263&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K263" s="9" t="str" cm="1">
@@ -11380,7 +11379,7 @@
         <v>1.4</v>
       </c>
       <c r="J264" s="9" t="str" cm="1">
-        <f t="array" ref="J264">_xlfn.IFS(I264&gt;=3.7,"A",I264&gt;=3.3,"B",I264&gt;=2.9,"C",I264&gt;=2.6,"D",I264&lt;=2.5,"E")</f>
+        <f t="array" ref="J264">_xlfn.IFS(I264&gt;=3.7,"A",I264&gt;=3.3,"B",I264&gt;=2.8,"C",I264&gt;=2.5,"D",I264&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K264" s="9" t="str" cm="1">
@@ -11421,7 +11420,7 @@
         <v>1.4</v>
       </c>
       <c r="J265" s="9" t="str" cm="1">
-        <f t="array" ref="J265">_xlfn.IFS(I265&gt;=3.7,"A",I265&gt;=3.3,"B",I265&gt;=2.9,"C",I265&gt;=2.6,"D",I265&lt;=2.5,"E")</f>
+        <f t="array" ref="J265">_xlfn.IFS(I265&gt;=3.7,"A",I265&gt;=3.3,"B",I265&gt;=2.8,"C",I265&gt;=2.5,"D",I265&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K265" s="9" t="str" cm="1">
@@ -11462,7 +11461,7 @@
         <v>1.4</v>
       </c>
       <c r="J266" s="9" t="str" cm="1">
-        <f t="array" ref="J266">_xlfn.IFS(I266&gt;=3.7,"A",I266&gt;=3.3,"B",I266&gt;=2.9,"C",I266&gt;=2.6,"D",I266&lt;=2.5,"E")</f>
+        <f t="array" ref="J266">_xlfn.IFS(I266&gt;=3.7,"A",I266&gt;=3.3,"B",I266&gt;=2.8,"C",I266&gt;=2.5,"D",I266&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K266" s="9" t="str" cm="1">
@@ -11503,7 +11502,7 @@
         <v>1.3</v>
       </c>
       <c r="J267" s="9" t="str" cm="1">
-        <f t="array" ref="J267">_xlfn.IFS(I267&gt;=3.7,"A",I267&gt;=3.3,"B",I267&gt;=2.9,"C",I267&gt;=2.6,"D",I267&lt;=2.5,"E")</f>
+        <f t="array" ref="J267">_xlfn.IFS(I267&gt;=3.7,"A",I267&gt;=3.3,"B",I267&gt;=2.8,"C",I267&gt;=2.5,"D",I267&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K267" s="9" t="str" cm="1">
@@ -11544,7 +11543,7 @@
         <v>1.3</v>
       </c>
       <c r="J268" s="9" t="str" cm="1">
-        <f t="array" ref="J268">_xlfn.IFS(I268&gt;=3.7,"A",I268&gt;=3.3,"B",I268&gt;=2.9,"C",I268&gt;=2.6,"D",I268&lt;=2.5,"E")</f>
+        <f t="array" ref="J268">_xlfn.IFS(I268&gt;=3.7,"A",I268&gt;=3.3,"B",I268&gt;=2.8,"C",I268&gt;=2.5,"D",I268&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K268" s="9" t="str" cm="1">
@@ -11585,7 +11584,7 @@
         <v>1.3</v>
       </c>
       <c r="J269" s="9" t="str" cm="1">
-        <f t="array" ref="J269">_xlfn.IFS(I269&gt;=3.7,"A",I269&gt;=3.3,"B",I269&gt;=2.9,"C",I269&gt;=2.6,"D",I269&lt;=2.5,"E")</f>
+        <f t="array" ref="J269">_xlfn.IFS(I269&gt;=3.7,"A",I269&gt;=3.3,"B",I269&gt;=2.8,"C",I269&gt;=2.5,"D",I269&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K269" s="9" t="str" cm="1">
@@ -11626,7 +11625,7 @@
         <v>1.3</v>
       </c>
       <c r="J270" s="9" t="str" cm="1">
-        <f t="array" ref="J270">_xlfn.IFS(I270&gt;=3.7,"A",I270&gt;=3.3,"B",I270&gt;=2.9,"C",I270&gt;=2.6,"D",I270&lt;=2.5,"E")</f>
+        <f t="array" ref="J270">_xlfn.IFS(I270&gt;=3.7,"A",I270&gt;=3.3,"B",I270&gt;=2.8,"C",I270&gt;=2.5,"D",I270&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K270" s="9" t="str" cm="1">
@@ -11667,7 +11666,7 @@
         <v>1.3</v>
       </c>
       <c r="J271" s="9" t="str" cm="1">
-        <f t="array" ref="J271">_xlfn.IFS(I271&gt;=3.7,"A",I271&gt;=3.3,"B",I271&gt;=2.9,"C",I271&gt;=2.6,"D",I271&lt;=2.5,"E")</f>
+        <f t="array" ref="J271">_xlfn.IFS(I271&gt;=3.7,"A",I271&gt;=3.3,"B",I271&gt;=2.8,"C",I271&gt;=2.5,"D",I271&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K271" s="9" t="str" cm="1">
@@ -11708,7 +11707,7 @@
         <v>1.2</v>
       </c>
       <c r="J272" s="9" t="str" cm="1">
-        <f t="array" ref="J272">_xlfn.IFS(I272&gt;=3.7,"A",I272&gt;=3.3,"B",I272&gt;=2.9,"C",I272&gt;=2.6,"D",I272&lt;=2.5,"E")</f>
+        <f t="array" ref="J272">_xlfn.IFS(I272&gt;=3.7,"A",I272&gt;=3.3,"B",I272&gt;=2.8,"C",I272&gt;=2.5,"D",I272&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K272" s="9" t="str" cm="1">
@@ -11749,7 +11748,7 @@
         <v>1.2</v>
       </c>
       <c r="J273" s="9" t="str" cm="1">
-        <f t="array" ref="J273">_xlfn.IFS(I273&gt;=3.7,"A",I273&gt;=3.3,"B",I273&gt;=2.9,"C",I273&gt;=2.6,"D",I273&lt;=2.5,"E")</f>
+        <f t="array" ref="J273">_xlfn.IFS(I273&gt;=3.7,"A",I273&gt;=3.3,"B",I273&gt;=2.8,"C",I273&gt;=2.5,"D",I273&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K273" s="9" t="str" cm="1">
@@ -11790,7 +11789,7 @@
         <v>1.2</v>
       </c>
       <c r="J274" s="9" t="str" cm="1">
-        <f t="array" ref="J274">_xlfn.IFS(I274&gt;=3.7,"A",I274&gt;=3.3,"B",I274&gt;=2.9,"C",I274&gt;=2.6,"D",I274&lt;=2.5,"E")</f>
+        <f t="array" ref="J274">_xlfn.IFS(I274&gt;=3.7,"A",I274&gt;=3.3,"B",I274&gt;=2.8,"C",I274&gt;=2.5,"D",I274&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K274" s="9" t="str" cm="1">
@@ -11831,7 +11830,7 @@
         <v>1.2</v>
       </c>
       <c r="J275" s="9" t="str" cm="1">
-        <f t="array" ref="J275">_xlfn.IFS(I275&gt;=3.7,"A",I275&gt;=3.3,"B",I275&gt;=2.9,"C",I275&gt;=2.6,"D",I275&lt;=2.5,"E")</f>
+        <f t="array" ref="J275">_xlfn.IFS(I275&gt;=3.7,"A",I275&gt;=3.3,"B",I275&gt;=2.8,"C",I275&gt;=2.5,"D",I275&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K275" s="9" t="str" cm="1">
@@ -11872,7 +11871,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J276" s="9" t="str" cm="1">
-        <f t="array" ref="J276">_xlfn.IFS(I276&gt;=3.7,"A",I276&gt;=3.3,"B",I276&gt;=2.9,"C",I276&gt;=2.6,"D",I276&lt;=2.5,"E")</f>
+        <f t="array" ref="J276">_xlfn.IFS(I276&gt;=3.7,"A",I276&gt;=3.3,"B",I276&gt;=2.8,"C",I276&gt;=2.5,"D",I276&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K276" s="9" t="str" cm="1">
@@ -11913,7 +11912,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J277" s="9" t="str" cm="1">
-        <f t="array" ref="J277">_xlfn.IFS(I277&gt;=3.7,"A",I277&gt;=3.3,"B",I277&gt;=2.9,"C",I277&gt;=2.6,"D",I277&lt;=2.5,"E")</f>
+        <f t="array" ref="J277">_xlfn.IFS(I277&gt;=3.7,"A",I277&gt;=3.3,"B",I277&gt;=2.8,"C",I277&gt;=2.5,"D",I277&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K277" s="9" t="str" cm="1">
@@ -11954,7 +11953,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J278" s="9" t="str" cm="1">
-        <f t="array" ref="J278">_xlfn.IFS(I278&gt;=3.7,"A",I278&gt;=3.3,"B",I278&gt;=2.9,"C",I278&gt;=2.6,"D",I278&lt;=2.5,"E")</f>
+        <f t="array" ref="J278">_xlfn.IFS(I278&gt;=3.7,"A",I278&gt;=3.3,"B",I278&gt;=2.8,"C",I278&gt;=2.5,"D",I278&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K278" s="9" t="str" cm="1">
@@ -11995,7 +11994,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J279" s="9" t="str" cm="1">
-        <f t="array" ref="J279">_xlfn.IFS(I279&gt;=3.7,"A",I279&gt;=3.3,"B",I279&gt;=2.9,"C",I279&gt;=2.6,"D",I279&lt;=2.5,"E")</f>
+        <f t="array" ref="J279">_xlfn.IFS(I279&gt;=3.7,"A",I279&gt;=3.3,"B",I279&gt;=2.8,"C",I279&gt;=2.5,"D",I279&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K279" s="9" t="str" cm="1">
@@ -12036,7 +12035,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J280" s="9" t="str" cm="1">
-        <f t="array" ref="J280">_xlfn.IFS(I280&gt;=3.7,"A",I280&gt;=3.3,"B",I280&gt;=2.9,"C",I280&gt;=2.6,"D",I280&lt;=2.5,"E")</f>
+        <f t="array" ref="J280">_xlfn.IFS(I280&gt;=3.7,"A",I280&gt;=3.3,"B",I280&gt;=2.8,"C",I280&gt;=2.5,"D",I280&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K280" s="9" t="str" cm="1">
@@ -12077,7 +12076,7 @@
         <v>1</v>
       </c>
       <c r="J281" s="9" t="str" cm="1">
-        <f t="array" ref="J281">_xlfn.IFS(I281&gt;=3.7,"A",I281&gt;=3.3,"B",I281&gt;=2.9,"C",I281&gt;=2.6,"D",I281&lt;=2.5,"E")</f>
+        <f t="array" ref="J281">_xlfn.IFS(I281&gt;=3.7,"A",I281&gt;=3.3,"B",I281&gt;=2.8,"C",I281&gt;=2.5,"D",I281&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K281" s="9" t="str" cm="1">
@@ -12118,7 +12117,7 @@
         <v>1</v>
       </c>
       <c r="J282" s="9" t="str" cm="1">
-        <f t="array" ref="J282">_xlfn.IFS(I282&gt;=3.7,"A",I282&gt;=3.3,"B",I282&gt;=2.9,"C",I282&gt;=2.6,"D",I282&lt;=2.5,"E")</f>
+        <f t="array" ref="J282">_xlfn.IFS(I282&gt;=3.7,"A",I282&gt;=3.3,"B",I282&gt;=2.8,"C",I282&gt;=2.5,"D",I282&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K282" s="9" t="str" cm="1">
@@ -12159,7 +12158,7 @@
         <v>1</v>
       </c>
       <c r="J283" s="9" t="str" cm="1">
-        <f t="array" ref="J283">_xlfn.IFS(I283&gt;=3.7,"A",I283&gt;=3.3,"B",I283&gt;=2.9,"C",I283&gt;=2.6,"D",I283&lt;=2.5,"E")</f>
+        <f t="array" ref="J283">_xlfn.IFS(I283&gt;=3.7,"A",I283&gt;=3.3,"B",I283&gt;=2.8,"C",I283&gt;=2.5,"D",I283&lt;=2.4,"E")</f>
         <v>E</v>
       </c>
       <c r="K283" s="9" t="str" cm="1">

</xml_diff>